<commit_message>
Proj v1, ready. port_draw in multiple T classes. pb v1. proj v1, ready. WinMain v3.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="711">
   <si>
     <t>Function</t>
   </si>
@@ -2126,6 +2126,27 @@
   </si>
   <si>
     <t>sub/bad regs</t>
+  </si>
+  <si>
+    <t>TEdgeSegment</t>
+  </si>
+  <si>
+    <t>Tline</t>
+  </si>
+  <si>
+    <t>TCircle</t>
+  </si>
+  <si>
+    <t>TCollisionComponent</t>
+  </si>
+  <si>
+    <t>proj</t>
+  </si>
+  <si>
+    <t>timer</t>
+  </si>
+  <si>
+    <t>inp</t>
   </si>
 </sst>
 </file>
@@ -2669,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B487" sqref="B487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2689,15 +2710,15 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:151</v>
+        <v>Done:174</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
-        <v>Inp:5</v>
+        <v>Inp:7</v>
       </c>
       <c r="D1" s="8" t="str">
         <f t="array" ref="D1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:20</v>
+        <v>Classes:26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3249,10 +3270,14 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="7" t="s">
+      <c r="A56" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C56" s="10"/>
+      <c r="D56" s="11" t="s">
         <v>454</v>
       </c>
     </row>
@@ -4179,10 +4204,14 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
-      <c r="C151" s="5"/>
-      <c r="D151" s="7" t="s">
+      <c r="A151" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C151" s="10"/>
+      <c r="D151" s="11" t="s">
         <v>500</v>
       </c>
     </row>
@@ -4283,10 +4312,14 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="2"/>
-      <c r="B164" s="2"/>
-      <c r="C164" s="5"/>
-      <c r="D164" s="7" t="s">
+      <c r="A164" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C164" s="10"/>
+      <c r="D164" s="11" t="s">
         <v>502</v>
       </c>
     </row>
@@ -4539,10 +4572,14 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="2"/>
-      <c r="B189" s="2"/>
-      <c r="C189" s="5"/>
-      <c r="D189" s="7" t="s">
+      <c r="A189" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="B189" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C189" s="10"/>
+      <c r="D189" s="11" t="s">
         <v>519</v>
       </c>
     </row>
@@ -4761,10 +4798,14 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="2"/>
-      <c r="B213" s="2"/>
-      <c r="C213" s="5"/>
-      <c r="D213" s="7" t="s">
+      <c r="A213" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="B213" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C213" s="10"/>
+      <c r="D213" s="11" t="s">
         <v>531</v>
       </c>
     </row>
@@ -5276,7 +5317,9 @@
       <c r="A259" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="B259" s="15"/>
+      <c r="B259" s="15" t="s">
+        <v>669</v>
+      </c>
       <c r="C259" s="18"/>
       <c r="D259" s="12" t="s">
         <v>576</v>
@@ -5461,58 +5504,86 @@
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A278" s="2"/>
-      <c r="B278" s="2"/>
-      <c r="C278" s="5"/>
-      <c r="D278" s="7" t="s">
+      <c r="A278" s="21" t="s">
+        <v>708</v>
+      </c>
+      <c r="B278" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C278" s="21"/>
+      <c r="D278" s="22" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A279" s="2"/>
-      <c r="B279" s="2"/>
-      <c r="C279" s="5"/>
-      <c r="D279" s="7" t="s">
+      <c r="A279" s="21" t="s">
+        <v>708</v>
+      </c>
+      <c r="B279" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C279" s="21"/>
+      <c r="D279" s="22" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A280" s="2"/>
-      <c r="B280" s="2"/>
-      <c r="C280" s="5"/>
-      <c r="D280" s="7" t="s">
+      <c r="A280" s="21" t="s">
+        <v>708</v>
+      </c>
+      <c r="B280" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C280" s="21"/>
+      <c r="D280" s="22" t="s">
         <v>595</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A281" s="2"/>
-      <c r="B281" s="2"/>
-      <c r="C281" s="5"/>
-      <c r="D281" s="7" t="s">
+      <c r="A281" s="21" t="s">
+        <v>708</v>
+      </c>
+      <c r="B281" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C281" s="21"/>
+      <c r="D281" s="22" t="s">
         <v>596</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A282" s="2"/>
-      <c r="B282" s="2"/>
-      <c r="C282" s="5"/>
-      <c r="D282" s="7" t="s">
+      <c r="A282" s="21" t="s">
+        <v>708</v>
+      </c>
+      <c r="B282" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C282" s="21"/>
+      <c r="D282" s="22" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A283" s="2"/>
-      <c r="B283" s="2"/>
-      <c r="C283" s="5"/>
-      <c r="D283" s="7" t="s">
+      <c r="A283" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="B283" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C283" s="10"/>
+      <c r="D283" s="11" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A284" s="2"/>
-      <c r="B284" s="2"/>
-      <c r="C284" s="5"/>
-      <c r="D284" s="7" t="s">
+      <c r="A284" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="B284" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C284" s="10"/>
+      <c r="D284" s="11" t="s">
         <v>599</v>
       </c>
     </row>
@@ -6651,74 +6722,102 @@
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A412" s="2"/>
-      <c r="B412" s="2"/>
-      <c r="C412" s="5"/>
-      <c r="D412" s="7" t="s">
+      <c r="A412" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="B412" s="9"/>
+      <c r="C412" s="10"/>
+      <c r="D412" s="11" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A413" s="2"/>
-      <c r="B413" s="2"/>
-      <c r="C413" s="5"/>
-      <c r="D413" s="7" t="s">
+      <c r="A413" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="B413" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C413" s="10"/>
+      <c r="D413" s="11" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A414" s="2"/>
-      <c r="B414" s="2"/>
-      <c r="C414" s="5"/>
-      <c r="D414" s="7" t="s">
+      <c r="A414" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="B414" s="9"/>
+      <c r="C414" s="10"/>
+      <c r="D414" s="11" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A415" s="2"/>
-      <c r="B415" s="2"/>
-      <c r="C415" s="5"/>
-      <c r="D415" s="7" t="s">
+      <c r="A415" s="9" t="s">
+        <v>706</v>
+      </c>
+      <c r="B415" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C415" s="10"/>
+      <c r="D415" s="11" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A416" s="2"/>
-      <c r="B416" s="2"/>
-      <c r="C416" s="5"/>
-      <c r="D416" s="7" t="s">
+      <c r="A416" s="21" t="s">
+        <v>707</v>
+      </c>
+      <c r="B416" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C416" s="21"/>
+      <c r="D416" s="22" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A417" s="2"/>
-      <c r="B417" s="2"/>
-      <c r="C417" s="5"/>
-      <c r="D417" s="7" t="s">
+      <c r="A417" s="21" t="s">
+        <v>707</v>
+      </c>
+      <c r="B417" s="21"/>
+      <c r="C417" s="21"/>
+      <c r="D417" s="22" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A418" s="2"/>
-      <c r="B418" s="2"/>
-      <c r="C418" s="5"/>
-      <c r="D418" s="7" t="s">
+      <c r="A418" s="21" t="s">
+        <v>707</v>
+      </c>
+      <c r="B418" s="21"/>
+      <c r="C418" s="21"/>
+      <c r="D418" s="22" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A419" s="2"/>
-      <c r="B419" s="2"/>
-      <c r="C419" s="5"/>
-      <c r="D419" s="7" t="s">
+      <c r="A419" s="21" t="s">
+        <v>707</v>
+      </c>
+      <c r="B419" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C419" s="21"/>
+      <c r="D419" s="22" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A420" s="2"/>
-      <c r="B420" s="2"/>
-      <c r="C420" s="5"/>
-      <c r="D420" s="7" t="s">
+      <c r="A420" s="21" t="s">
+        <v>707</v>
+      </c>
+      <c r="B420" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C420" s="21"/>
+      <c r="D420" s="22" t="s">
         <v>207</v>
       </c>
     </row>
@@ -6987,10 +7086,14 @@
       </c>
     </row>
     <row r="454" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A454" s="2"/>
-      <c r="B454" s="2"/>
-      <c r="C454" s="5"/>
-      <c r="D454" s="7" t="s">
+      <c r="A454" s="9" t="s">
+        <v>704</v>
+      </c>
+      <c r="B454" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C454" s="10"/>
+      <c r="D454" s="11" t="s">
         <v>243</v>
       </c>
     </row>
@@ -7251,42 +7354,54 @@
       </c>
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A487" s="2"/>
-      <c r="B487" s="2"/>
-      <c r="C487" s="5"/>
-      <c r="D487" s="7" t="s">
+      <c r="A487" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="B487" s="9"/>
+      <c r="C487" s="10"/>
+      <c r="D487" s="11" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="488" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A488" s="2"/>
-      <c r="B488" s="2"/>
-      <c r="C488" s="5"/>
-      <c r="D488" s="7" t="s">
+      <c r="A488" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="B488" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="C488" s="10"/>
+      <c r="D488" s="11" t="s">
         <v>649</v>
       </c>
     </row>
     <row r="489" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A489" s="2"/>
-      <c r="B489" s="2"/>
-      <c r="C489" s="5"/>
-      <c r="D489" s="7" t="s">
+      <c r="A489" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="B489" s="9"/>
+      <c r="C489" s="10"/>
+      <c r="D489" s="11" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A490" s="2"/>
-      <c r="B490" s="2"/>
-      <c r="C490" s="5"/>
-      <c r="D490" s="7" t="s">
+      <c r="A490" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="B490" s="9"/>
+      <c r="C490" s="10"/>
+      <c r="D490" s="11" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A491" s="2"/>
-      <c r="B491" s="2"/>
-      <c r="C491" s="5"/>
-      <c r="D491" s="7" t="s">
+      <c r="A491" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="B491" s="9"/>
+      <c r="C491" s="10"/>
+      <c r="D491" s="11" t="s">
         <v>652</v>
       </c>
     </row>
@@ -7611,50 +7726,70 @@
       </c>
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A532" s="2"/>
-      <c r="B532" s="2"/>
-      <c r="C532" s="5"/>
-      <c r="D532" s="7" t="s">
+      <c r="A532" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="B532" s="9"/>
+      <c r="C532" s="10"/>
+      <c r="D532" s="11" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A533" s="2"/>
-      <c r="B533" s="2"/>
-      <c r="C533" s="5"/>
-      <c r="D533" s="7" t="s">
+      <c r="A533" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="B533" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C533" s="10"/>
+      <c r="D533" s="11" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A534" s="2"/>
-      <c r="B534" s="2"/>
-      <c r="C534" s="5"/>
-      <c r="D534" s="7" t="s">
+      <c r="A534" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="B534" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C534" s="10"/>
+      <c r="D534" s="11" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A535" s="2"/>
-      <c r="B535" s="2"/>
-      <c r="C535" s="5"/>
-      <c r="D535" s="7" t="s">
+      <c r="A535" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="B535" s="9"/>
+      <c r="C535" s="10"/>
+      <c r="D535" s="11" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A536" s="2"/>
-      <c r="B536" s="2"/>
-      <c r="C536" s="5"/>
-      <c r="D536" s="7" t="s">
+      <c r="A536" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="B536" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C536" s="10"/>
+      <c r="D536" s="11" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A537" s="2"/>
-      <c r="B537" s="2"/>
-      <c r="C537" s="5"/>
-      <c r="D537" s="7" t="s">
+      <c r="A537" s="9" t="s">
+        <v>705</v>
+      </c>
+      <c r="B537" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C537" s="10"/>
+      <c r="D537" s="11" t="s">
         <v>317</v>
       </c>
     </row>
@@ -7874,7 +8009,9 @@
       <c r="A558" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B558" s="15"/>
+      <c r="B558" s="15" t="s">
+        <v>668</v>
+      </c>
       <c r="C558" s="18"/>
       <c r="D558" s="12" t="s">
         <v>339</v>

</xml_diff>

<commit_message>
TTextBoxMessage v1, ready. TTextBox v1.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="712">
   <si>
     <t>Function</t>
   </si>
@@ -2147,6 +2147,9 @@
   </si>
   <si>
     <t>inp</t>
+  </si>
+  <si>
+    <t>TTextBoxMessage</t>
   </si>
 </sst>
 </file>
@@ -2691,7 +2694,7 @@
   <dimension ref="A1:D669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,15 +2713,15 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:189</v>
+        <v>Done:200</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
-        <v>Inp:6</v>
+        <v>Inp:7</v>
       </c>
       <c r="D1" s="8" t="str">
         <f t="array" ref="D1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:26</v>
+        <v>Classes:27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4084,10 +4087,14 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="2"/>
-      <c r="B136" s="2"/>
-      <c r="C136" s="5"/>
-      <c r="D136" s="7" t="s">
+      <c r="A136" s="9" t="s">
+        <v>696</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>668</v>
+      </c>
+      <c r="C136" s="10"/>
+      <c r="D136" s="11" t="s">
         <v>492</v>
       </c>
     </row>
@@ -8449,7 +8456,9 @@
       <c r="A608" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="B608" s="9"/>
+      <c r="B608" s="9" t="s">
+        <v>668</v>
+      </c>
       <c r="C608" s="10"/>
       <c r="D608" s="11" t="s">
         <v>395</v>
@@ -8459,7 +8468,9 @@
       <c r="A609" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="B609" s="9"/>
+      <c r="B609" s="9" t="s">
+        <v>668</v>
+      </c>
       <c r="C609" s="10"/>
       <c r="D609" s="11" t="s">
         <v>396</v>
@@ -8469,7 +8480,9 @@
       <c r="A610" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="B610" s="9"/>
+      <c r="B610" s="9" t="s">
+        <v>668</v>
+      </c>
       <c r="C610" s="10"/>
       <c r="D610" s="11" t="s">
         <v>389</v>
@@ -8479,7 +8492,9 @@
       <c r="A611" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="B611" s="9"/>
+      <c r="B611" s="9" t="s">
+        <v>668</v>
+      </c>
       <c r="C611" s="10"/>
       <c r="D611" s="11" t="s">
         <v>390</v>
@@ -8489,7 +8504,9 @@
       <c r="A612" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="B612" s="9"/>
+      <c r="B612" s="9" t="s">
+        <v>669</v>
+      </c>
       <c r="C612" s="10"/>
       <c r="D612" s="11" t="s">
         <v>391</v>
@@ -8511,7 +8528,9 @@
       <c r="A614" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="B614" s="9"/>
+      <c r="B614" s="9" t="s">
+        <v>668</v>
+      </c>
       <c r="C614" s="10"/>
       <c r="D614" s="11" t="s">
         <v>394</v>
@@ -8521,41 +8540,59 @@
       <c r="A615" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="B615" s="9"/>
+      <c r="B615" s="9" t="s">
+        <v>668</v>
+      </c>
       <c r="C615" s="10"/>
       <c r="D615" s="11" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="616" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A616" s="2"/>
-      <c r="B616" s="2"/>
-      <c r="C616" s="5"/>
-      <c r="D616" s="7" t="s">
+      <c r="A616" s="21" t="s">
+        <v>711</v>
+      </c>
+      <c r="B616" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C616" s="21"/>
+      <c r="D616" s="22" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="617" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A617" s="2"/>
-      <c r="B617" s="2"/>
-      <c r="C617" s="5"/>
-      <c r="D617" s="7" t="s">
+      <c r="A617" s="21" t="s">
+        <v>711</v>
+      </c>
+      <c r="B617" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C617" s="21"/>
+      <c r="D617" s="22" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="618" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A618" s="2"/>
-      <c r="B618" s="2"/>
-      <c r="C618" s="5"/>
-      <c r="D618" s="7" t="s">
+      <c r="A618" s="21" t="s">
+        <v>711</v>
+      </c>
+      <c r="B618" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C618" s="21"/>
+      <c r="D618" s="22" t="s">
         <v>399</v>
       </c>
     </row>
     <row r="619" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A619" s="2"/>
-      <c r="B619" s="2"/>
-      <c r="C619" s="5"/>
-      <c r="D619" s="7" t="s">
+      <c r="A619" s="21" t="s">
+        <v>711</v>
+      </c>
+      <c r="B619" s="21" t="s">
+        <v>668</v>
+      </c>
+      <c r="C619" s="21"/>
+      <c r="D619" s="22" t="s">
         <v>398</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added icon, textbox font. TTextBox ready.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="713">
   <si>
     <t>Function</t>
   </si>
@@ -2676,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A249" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C262" sqref="C262"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2697,15 +2697,15 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:213</v>
+        <v>Done:216</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
-        <v>Inp:7</v>
+        <v>Inp:6</v>
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.22397303097382518</v>
+        <v>0.23400192635901249</v>
       </c>
       <c r="E1" s="7" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
@@ -7084,7 +7084,9 @@
       <c r="A333" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="B333" s="8"/>
+      <c r="B333" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C333" s="8"/>
       <c r="D333" s="13">
         <v>538</v>
@@ -7123,7 +7125,9 @@
       <c r="A336" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="B336" s="8"/>
+      <c r="B336" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C336" s="8"/>
       <c r="D336" s="13">
         <v>64</v>
@@ -10362,7 +10366,7 @@
         <v>698</v>
       </c>
       <c r="B612" s="8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C612" s="8"/>
       <c r="D612" s="13">

</xml_diff>

<commit_message>
score, high_score ready. Added dialog rc.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="714">
   <si>
     <t>Function</t>
   </si>
@@ -2153,6 +2153,9 @@
   </si>
   <si>
     <t>TRamp</t>
+  </si>
+  <si>
+    <t>high_score</t>
   </si>
 </sst>
 </file>
@@ -2196,7 +2199,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2216,6 +2219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2277,7 +2286,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2309,6 +2318,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2677,7 +2693,7 @@
   <dimension ref="A1:E669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2697,7 +2713,7 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:216</v>
+        <v>Done:231</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
@@ -2705,11 +2721,11 @@
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.23400192635901249</v>
+        <v>0.25509893712296594</v>
       </c>
       <c r="E1" s="7" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:28</v>
+        <v>Classes:29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4519,79 +4535,107 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
-      <c r="D139" s="15">
+      <c r="A139" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B139" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C139" s="16"/>
+      <c r="D139" s="17">
         <v>31</v>
       </c>
-      <c r="E139" s="6" t="s">
+      <c r="E139" s="18" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="15">
+      <c r="A140" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B140" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C140" s="16"/>
+      <c r="D140" s="17">
         <v>40</v>
       </c>
-      <c r="E140" s="6" t="s">
+      <c r="E140" s="18" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="15">
+      <c r="A141" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B141" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C141" s="16"/>
+      <c r="D141" s="17">
         <v>103</v>
       </c>
-      <c r="E141" s="6" t="s">
+      <c r="E141" s="18" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="15">
+      <c r="A142" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B142" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C142" s="16"/>
+      <c r="D142" s="17">
         <v>362</v>
       </c>
-      <c r="E142" s="6" t="s">
+      <c r="E142" s="18" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="15">
+      <c r="A143" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B143" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C143" s="16"/>
+      <c r="D143" s="17">
         <v>269</v>
       </c>
-      <c r="E143" s="6" t="s">
+      <c r="E143" s="18" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" s="2"/>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
-      <c r="D144" s="15">
+      <c r="A144" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B144" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C144" s="16"/>
+      <c r="D144" s="17">
         <v>600</v>
       </c>
-      <c r="E144" s="6" t="s">
+      <c r="E144" s="18" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
-      <c r="D145" s="15">
+      <c r="A145" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B145" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C145" s="16"/>
+      <c r="D145" s="17">
         <v>114</v>
       </c>
-      <c r="E145" s="6" t="s">
+      <c r="E145" s="18" t="s">
         <v>499</v>
       </c>
     </row>
@@ -7056,7 +7100,9 @@
       <c r="A331" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="B331" s="8"/>
+      <c r="B331" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C331" s="8"/>
       <c r="D331" s="13">
         <v>126</v>
@@ -7099,7 +7145,9 @@
       <c r="A334" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="B334" s="8"/>
+      <c r="B334" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C334" s="8"/>
       <c r="D334" s="13">
         <v>28</v>
@@ -7112,7 +7160,9 @@
       <c r="A335" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="B335" s="8"/>
+      <c r="B335" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C335" s="8"/>
       <c r="D335" s="13">
         <v>324</v>
@@ -7140,7 +7190,9 @@
       <c r="A337" s="8" t="s">
         <v>687</v>
       </c>
-      <c r="B337" s="8"/>
+      <c r="B337" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C337" s="8"/>
       <c r="D337" s="13">
         <v>243</v>
@@ -7150,13 +7202,17 @@
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A338" s="2"/>
-      <c r="B338" s="2"/>
-      <c r="C338" s="2"/>
-      <c r="D338" s="15">
+      <c r="A338" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B338" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C338" s="16"/>
+      <c r="D338" s="17">
         <v>26</v>
       </c>
-      <c r="E338" s="6" t="s">
+      <c r="E338" s="18" t="s">
         <v>627</v>
       </c>
     </row>
@@ -7282,35 +7338,47 @@
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A350" s="2"/>
-      <c r="B350" s="2"/>
-      <c r="C350" s="2"/>
-      <c r="D350" s="15">
+      <c r="A350" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B350" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C350" s="16"/>
+      <c r="D350" s="17">
         <v>85</v>
       </c>
-      <c r="E350" s="6" t="s">
+      <c r="E350" s="18" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A351" s="2"/>
-      <c r="B351" s="2"/>
-      <c r="C351" s="2"/>
-      <c r="D351" s="15">
+      <c r="A351" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B351" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C351" s="16"/>
+      <c r="D351" s="17">
         <v>59</v>
       </c>
-      <c r="E351" s="6" t="s">
+      <c r="E351" s="18" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A352" s="2"/>
-      <c r="B352" s="2"/>
-      <c r="C352" s="2"/>
-      <c r="D352" s="15">
+      <c r="A352" s="16" t="s">
+        <v>713</v>
+      </c>
+      <c r="B352" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C352" s="16"/>
+      <c r="D352" s="17">
         <v>87</v>
       </c>
-      <c r="E352" s="6" t="s">
+      <c r="E352" s="18" t="s">
         <v>630</v>
       </c>
     </row>

</xml_diff>

<commit_message>
key mapper dialog, ready.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="714">
   <si>
     <t>Function</t>
   </si>
@@ -2713,15 +2713,15 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:231</v>
+        <v>Done:233</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
-        <v>Inp:6</v>
+        <v>Inp:5</v>
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.25509893712296594</v>
+        <v>0.27063654336842463</v>
       </c>
       <c r="E1" s="7" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
@@ -4428,13 +4428,17 @@
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="15">
+      <c r="A130" s="16" t="s">
+        <v>680</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C130" s="16"/>
+      <c r="D130" s="17">
         <v>63</v>
       </c>
-      <c r="E130" s="6" t="s">
+      <c r="E130" s="18" t="s">
         <v>491</v>
       </c>
     </row>
@@ -4736,7 +4740,7 @@
         <v>680</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C154" s="8"/>
       <c r="D154" s="13">

</xml_diff>

<commit_message>
TBall, nudge v1, ready. render occlude list.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="718">
   <si>
     <t>Function</t>
   </si>
@@ -2162,6 +2162,12 @@
   </si>
   <si>
     <t>TTableLayer</t>
+  </si>
+  <si>
+    <t>nudge</t>
+  </si>
+  <si>
+    <t>Tball</t>
   </si>
 </sst>
 </file>
@@ -2205,7 +2211,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2231,6 +2237,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2292,7 +2304,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2330,6 +2342,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2401,6 +2420,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2699,7 +2723,7 @@
   <dimension ref="A1:E669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2719,19 +2743,19 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:247</v>
+        <v>Done:268</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
-        <v>Inp:6</v>
+        <v>Inp:4</v>
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.30274252690988357</v>
+        <v>0.33174774835668058</v>
       </c>
       <c r="E1" s="7" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:31</v>
+        <v>Classes:33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3306,13 +3330,17 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="15">
+      <c r="A44" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C44" s="8"/>
+      <c r="D44" s="13">
         <v>286</v>
       </c>
-      <c r="E44" s="6" t="s">
+      <c r="E44" s="9" t="s">
         <v>447</v>
       </c>
     </row>
@@ -5516,46 +5544,62 @@
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214" s="2"/>
-      <c r="B214" s="2"/>
-      <c r="C214" s="2"/>
-      <c r="D214" s="15">
+      <c r="A214" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="B214" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C214" s="19"/>
+      <c r="D214" s="20">
         <v>282</v>
       </c>
-      <c r="E214" s="6" t="s">
+      <c r="E214" s="21" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" s="2"/>
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
-      <c r="D215" s="15">
+      <c r="A215" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="B215" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C215" s="19"/>
+      <c r="D215" s="20">
         <v>77</v>
       </c>
-      <c r="E215" s="6" t="s">
+      <c r="E215" s="21" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" s="2"/>
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
-      <c r="D216" s="15">
+      <c r="A216" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="B216" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C216" s="19"/>
+      <c r="D216" s="20">
         <v>77</v>
       </c>
-      <c r="E216" s="6" t="s">
+      <c r="E216" s="21" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A217" s="2"/>
-      <c r="B217" s="2"/>
-      <c r="C217" s="2"/>
-      <c r="D217" s="15">
+      <c r="A217" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="B217" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C217" s="19"/>
+      <c r="D217" s="20">
         <v>73</v>
       </c>
-      <c r="E217" s="6" t="s">
+      <c r="E217" s="21" t="s">
         <v>535</v>
       </c>
     </row>
@@ -6073,7 +6117,9 @@
       <c r="A252" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="B252" s="11"/>
+      <c r="B252" s="11" t="s">
+        <v>668</v>
+      </c>
       <c r="C252" s="11"/>
       <c r="D252" s="14">
         <v>60</v>
@@ -6086,7 +6132,9 @@
       <c r="A253" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="B253" s="11"/>
+      <c r="B253" s="11" t="s">
+        <v>668</v>
+      </c>
       <c r="C253" s="11"/>
       <c r="D253" s="14">
         <v>73</v>
@@ -6140,7 +6188,9 @@
       <c r="A257" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="B257" s="11"/>
+      <c r="B257" s="11" t="s">
+        <v>669</v>
+      </c>
       <c r="C257" s="11"/>
       <c r="D257" s="14">
         <v>319</v>
@@ -6169,7 +6219,7 @@
         <v>683</v>
       </c>
       <c r="B259" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C259" s="11"/>
       <c r="D259" s="14">
@@ -6184,7 +6234,7 @@
         <v>683</v>
       </c>
       <c r="B260" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C260" s="11"/>
       <c r="D260" s="14">
@@ -6244,7 +6294,7 @@
         <v>683</v>
       </c>
       <c r="B264" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C264" s="11"/>
       <c r="D264" s="14">
@@ -6333,7 +6383,9 @@
       <c r="A270" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="B270" s="11"/>
+      <c r="B270" s="11" t="s">
+        <v>668</v>
+      </c>
       <c r="C270" s="11"/>
       <c r="D270" s="14">
         <v>48</v>
@@ -6359,7 +6411,9 @@
       <c r="A272" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="B272" s="11"/>
+      <c r="B272" s="11" t="s">
+        <v>668</v>
+      </c>
       <c r="C272" s="11"/>
       <c r="D272" s="14">
         <v>95</v>
@@ -6399,13 +6453,15 @@
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A275" s="2"/>
-      <c r="B275" s="2"/>
-      <c r="C275" s="2"/>
-      <c r="D275" s="15">
+      <c r="A275" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="B275" s="11"/>
+      <c r="C275" s="11"/>
+      <c r="D275" s="14">
         <v>854</v>
       </c>
-      <c r="E275" s="6" t="s">
+      <c r="E275" s="10" t="s">
         <v>592</v>
       </c>
     </row>
@@ -7923,57 +7979,77 @@
       </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A397" s="2"/>
-      <c r="B397" s="2"/>
-      <c r="C397" s="2"/>
-      <c r="D397" s="15">
+      <c r="A397" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="B397" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C397" s="8"/>
+      <c r="D397" s="13">
         <v>90</v>
       </c>
-      <c r="E397" s="6" t="s">
+      <c r="E397" s="9" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A398" s="2"/>
-      <c r="B398" s="2"/>
-      <c r="C398" s="2"/>
-      <c r="D398" s="15">
+      <c r="A398" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="B398" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C398" s="8"/>
+      <c r="D398" s="13">
         <v>103</v>
       </c>
-      <c r="E398" s="6" t="s">
+      <c r="E398" s="9" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A399" s="2"/>
-      <c r="B399" s="2"/>
-      <c r="C399" s="2"/>
-      <c r="D399" s="15">
+      <c r="A399" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="B399" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C399" s="8"/>
+      <c r="D399" s="13">
         <v>33</v>
       </c>
-      <c r="E399" s="6" t="s">
+      <c r="E399" s="9" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A400" s="2"/>
-      <c r="B400" s="2"/>
-      <c r="C400" s="2"/>
-      <c r="D400" s="15">
+      <c r="A400" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="B400" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C400" s="8"/>
+      <c r="D400" s="13">
         <v>165</v>
       </c>
-      <c r="E400" s="6" t="s">
+      <c r="E400" s="9" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A401" s="2"/>
-      <c r="B401" s="2"/>
-      <c r="C401" s="2"/>
-      <c r="D401" s="15">
+      <c r="A401" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="B401" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C401" s="8"/>
+      <c r="D401" s="13">
         <v>316</v>
       </c>
-      <c r="E401" s="6" t="s">
+      <c r="E401" s="9" t="s">
         <v>188</v>
       </c>
     </row>
@@ -10763,35 +10839,47 @@
       </c>
     </row>
     <row r="633" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A633" s="2"/>
-      <c r="B633" s="2"/>
-      <c r="C633" s="2"/>
-      <c r="D633" s="15">
+      <c r="A633" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="B633" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C633" s="19"/>
+      <c r="D633" s="20">
         <v>45</v>
       </c>
-      <c r="E633" s="6" t="s">
+      <c r="E633" s="21" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="634" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A634" s="2"/>
-      <c r="B634" s="2"/>
-      <c r="C634" s="2"/>
-      <c r="D634" s="15">
+      <c r="A634" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="B634" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C634" s="19"/>
+      <c r="D634" s="20">
         <v>45</v>
       </c>
-      <c r="E634" s="6" t="s">
+      <c r="E634" s="21" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="635" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A635" s="2"/>
-      <c r="B635" s="2"/>
-      <c r="C635" s="2"/>
-      <c r="D635" s="15">
+      <c r="A635" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="B635" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C635" s="19"/>
+      <c r="D635" s="20">
         <v>41</v>
       </c>
-      <c r="E635" s="6" t="s">
+      <c r="E635" s="21" t="s">
         <v>655</v>
       </c>
     </row>
@@ -10807,13 +10895,17 @@
       </c>
     </row>
     <row r="637" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A637" s="2"/>
-      <c r="B637" s="2"/>
-      <c r="C637" s="2"/>
-      <c r="D637" s="15">
+      <c r="A637" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="B637" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C637" s="8"/>
+      <c r="D637" s="13">
         <v>30</v>
       </c>
-      <c r="E637" s="6" t="s">
+      <c r="E637" s="9" t="s">
         <v>656</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TLight, TTimer, TSound, TComponentGroup ready.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="722">
   <si>
     <t>Function</t>
   </si>
@@ -2168,6 +2168,18 @@
   </si>
   <si>
     <t>Tball</t>
+  </si>
+  <si>
+    <t>TComponentGroup</t>
+  </si>
+  <si>
+    <t>TLight</t>
+  </si>
+  <si>
+    <t>TSound</t>
+  </si>
+  <si>
+    <t>TTimer</t>
   </si>
 </sst>
 </file>
@@ -2723,7 +2735,7 @@
   <dimension ref="A1:E669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2743,7 +2755,7 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:268</v>
+        <v>Done:287</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
@@ -2751,11 +2763,11 @@
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.33174774835668058</v>
+        <v>0.35149292823467781</v>
       </c>
       <c r="E1" s="7" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:33</v>
+        <v>Classes:37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3770,35 +3782,47 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="15">
+      <c r="A80" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C80" s="8"/>
+      <c r="D80" s="13">
         <v>59</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="E80" s="9" t="s">
         <v>460</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="15">
+      <c r="A81" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C81" s="8"/>
+      <c r="D81" s="13">
         <v>26</v>
       </c>
-      <c r="E81" s="6" t="s">
+      <c r="E81" s="9" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="15">
+      <c r="A82" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C82" s="8"/>
+      <c r="D82" s="13">
         <v>52</v>
       </c>
-      <c r="E82" s="6" t="s">
+      <c r="E82" s="9" t="s">
         <v>462</v>
       </c>
     </row>
@@ -8291,57 +8315,79 @@
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A421" s="2"/>
-      <c r="B421" s="2"/>
-      <c r="C421" s="2"/>
-      <c r="D421" s="15">
+      <c r="A421" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="B421" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C421" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="D421" s="13">
         <v>33</v>
       </c>
-      <c r="E421" s="6" t="s">
+      <c r="E421" s="9" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A422" s="2"/>
-      <c r="B422" s="2"/>
-      <c r="C422" s="2"/>
-      <c r="D422" s="15">
+      <c r="A422" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="B422" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C422" s="8"/>
+      <c r="D422" s="13">
         <v>44</v>
       </c>
-      <c r="E422" s="6" t="s">
+      <c r="E422" s="9" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A423" s="2"/>
-      <c r="B423" s="2"/>
-      <c r="C423" s="2"/>
-      <c r="D423" s="15">
+      <c r="A423" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="B423" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C423" s="8"/>
+      <c r="D423" s="13">
         <v>156</v>
       </c>
-      <c r="E423" s="6" t="s">
+      <c r="E423" s="9" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A424" s="2"/>
-      <c r="B424" s="2"/>
-      <c r="C424" s="2"/>
-      <c r="D424" s="15">
+      <c r="A424" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="B424" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C424" s="8"/>
+      <c r="D424" s="13">
         <v>24</v>
       </c>
-      <c r="E424" s="6" t="s">
+      <c r="E424" s="9" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A425" s="2"/>
-      <c r="B425" s="2"/>
-      <c r="C425" s="2"/>
-      <c r="D425" s="15">
+      <c r="A425" s="8" t="s">
+        <v>718</v>
+      </c>
+      <c r="B425" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C425" s="8"/>
+      <c r="D425" s="13">
         <v>128</v>
       </c>
-      <c r="E425" s="6" t="s">
+      <c r="E425" s="9" t="s">
         <v>212</v>
       </c>
     </row>
@@ -9250,57 +9296,77 @@
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A506" s="2"/>
-      <c r="B506" s="2"/>
-      <c r="C506" s="2"/>
-      <c r="D506" s="15">
+      <c r="A506" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B506" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C506" s="8"/>
+      <c r="D506" s="13">
         <v>1161</v>
       </c>
-      <c r="E506" s="6" t="s">
+      <c r="E506" s="9" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A507" s="2"/>
-      <c r="B507" s="2"/>
-      <c r="C507" s="2"/>
-      <c r="D507" s="15">
+      <c r="A507" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B507" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C507" s="8"/>
+      <c r="D507" s="13">
         <v>125</v>
       </c>
-      <c r="E507" s="6" t="s">
+      <c r="E507" s="9" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A508" s="2"/>
-      <c r="B508" s="2"/>
-      <c r="C508" s="2"/>
-      <c r="D508" s="15">
+      <c r="A508" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B508" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C508" s="8"/>
+      <c r="D508" s="13">
         <v>79</v>
       </c>
-      <c r="E508" s="6" t="s">
+      <c r="E508" s="9" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A509" s="2"/>
-      <c r="B509" s="2"/>
-      <c r="C509" s="2"/>
-      <c r="D509" s="15">
+      <c r="A509" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B509" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C509" s="8"/>
+      <c r="D509" s="13">
         <v>96</v>
       </c>
-      <c r="E509" s="6" t="s">
+      <c r="E509" s="9" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A510" s="2"/>
-      <c r="B510" s="2"/>
-      <c r="C510" s="2"/>
-      <c r="D510" s="15">
+      <c r="A510" s="8" t="s">
+        <v>719</v>
+      </c>
+      <c r="B510" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C510" s="8"/>
+      <c r="D510" s="13">
         <v>101</v>
       </c>
-      <c r="E510" s="6" t="s">
+      <c r="E510" s="9" t="s">
         <v>289</v>
       </c>
     </row>
@@ -10411,35 +10477,49 @@
       </c>
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A601" s="2"/>
-      <c r="B601" s="2"/>
-      <c r="C601" s="2"/>
-      <c r="D601" s="15">
+      <c r="A601" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="B601" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C601" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="D601" s="13">
         <v>33</v>
       </c>
-      <c r="E601" s="6" t="s">
+      <c r="E601" s="9" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A602" s="2"/>
-      <c r="B602" s="2"/>
-      <c r="C602" s="2"/>
-      <c r="D602" s="15">
+      <c r="A602" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="B602" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C602" s="8"/>
+      <c r="D602" s="13">
         <v>9</v>
       </c>
-      <c r="E602" s="6" t="s">
+      <c r="E602" s="9" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A603" s="2"/>
-      <c r="B603" s="2"/>
-      <c r="C603" s="2"/>
-      <c r="D603" s="15">
+      <c r="A603" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="B603" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C603" s="8"/>
+      <c r="D603" s="13">
         <v>57</v>
       </c>
-      <c r="E603" s="6" t="s">
+      <c r="E603" s="9" t="s">
         <v>383</v>
       </c>
     </row>
@@ -10684,35 +10764,47 @@
       </c>
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A620" s="2"/>
-      <c r="B620" s="2"/>
-      <c r="C620" s="2"/>
-      <c r="D620" s="15">
+      <c r="A620" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="B620" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C620" s="8"/>
+      <c r="D620" s="13">
         <v>92</v>
       </c>
-      <c r="E620" s="6" t="s">
+      <c r="E620" s="9" t="s">
         <v>401</v>
       </c>
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A621" s="2"/>
-      <c r="B621" s="2"/>
-      <c r="C621" s="2"/>
-      <c r="D621" s="15">
+      <c r="A621" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="B621" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C621" s="8"/>
+      <c r="D621" s="13">
         <v>24</v>
       </c>
-      <c r="E621" s="6" t="s">
+      <c r="E621" s="9" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A622" s="2"/>
-      <c r="B622" s="2"/>
-      <c r="C622" s="2"/>
-      <c r="D622" s="15">
+      <c r="A622" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="B622" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C622" s="8"/>
+      <c r="D622" s="13">
         <v>38</v>
       </c>
-      <c r="E622" s="6" t="s">
+      <c r="E622" s="9" t="s">
         <v>402</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pb, cheats ready. Collison v1, mouse fixed.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="722">
   <si>
     <t>Function</t>
   </si>
@@ -2316,7 +2316,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2361,6 +2361,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2734,8 +2741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E669"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A401" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E423" sqref="E423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2755,15 +2762,15 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:287</v>
+        <v>Done:297</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
-        <v>Inp:4</v>
+        <v>Inp:3</v>
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.35149292823467781</v>
+        <v>0.37678906368813264</v>
       </c>
       <c r="E1" s="7" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
@@ -3254,13 +3261,17 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="15">
+      <c r="A36" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="13">
         <v>246</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="9" t="s">
         <v>446</v>
       </c>
     </row>
@@ -3405,13 +3416,17 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="15">
+      <c r="A49" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20">
         <v>154</v>
       </c>
-      <c r="E49" s="6" t="s">
+      <c r="E49" s="21" t="s">
         <v>449</v>
       </c>
     </row>
@@ -6171,7 +6186,9 @@
       <c r="A254" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="B254" s="11"/>
+      <c r="B254" s="11" t="s">
+        <v>668</v>
+      </c>
       <c r="C254" s="11"/>
       <c r="D254" s="14">
         <v>269</v>
@@ -6184,7 +6201,9 @@
       <c r="A255" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="B255" s="11"/>
+      <c r="B255" s="11" t="s">
+        <v>668</v>
+      </c>
       <c r="C255" s="11"/>
       <c r="D255" s="14">
         <v>360</v>
@@ -6213,7 +6232,7 @@
         <v>683</v>
       </c>
       <c r="B257" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C257" s="11"/>
       <c r="D257" s="14">
@@ -6422,7 +6441,9 @@
       <c r="A271" s="11" t="s">
         <v>683</v>
       </c>
-      <c r="B271" s="11"/>
+      <c r="B271" s="11" t="s">
+        <v>668</v>
+      </c>
       <c r="C271" s="11"/>
       <c r="D271" s="14">
         <v>396</v>
@@ -6477,15 +6498,17 @@
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A275" s="11" t="s">
-        <v>683</v>
-      </c>
-      <c r="B275" s="11"/>
-      <c r="C275" s="11"/>
-      <c r="D275" s="14">
+      <c r="A275" s="22" t="s">
+        <v>714</v>
+      </c>
+      <c r="B275" s="22" t="s">
+        <v>668</v>
+      </c>
+      <c r="C275" s="22"/>
+      <c r="D275" s="23">
         <v>854</v>
       </c>
-      <c r="E275" s="10" t="s">
+      <c r="E275" s="24" t="s">
         <v>592</v>
       </c>
     </row>
@@ -7900,13 +7923,17 @@
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A388" s="2"/>
-      <c r="B388" s="2"/>
-      <c r="C388" s="2"/>
-      <c r="D388" s="15">
+      <c r="A388" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="B388" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C388" s="8"/>
+      <c r="D388" s="13">
         <v>61</v>
       </c>
-      <c r="E388" s="6" t="s">
+      <c r="E388" s="9" t="s">
         <v>638</v>
       </c>
     </row>
@@ -8262,7 +8289,9 @@
       <c r="A417" s="11" t="s">
         <v>707</v>
       </c>
-      <c r="B417" s="11"/>
+      <c r="B417" s="11" t="s">
+        <v>668</v>
+      </c>
       <c r="C417" s="11"/>
       <c r="D417" s="14">
         <v>159</v>
@@ -8275,7 +8304,9 @@
       <c r="A418" s="11" t="s">
         <v>707</v>
       </c>
-      <c r="B418" s="11"/>
+      <c r="B418" s="11" t="s">
+        <v>668</v>
+      </c>
       <c r="C418" s="11"/>
       <c r="D418" s="14">
         <v>176</v>

</xml_diff>

<commit_message>
TPlunger ready. TEdgeManager v1.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="725">
   <si>
     <t>Function</t>
   </si>
@@ -2180,6 +2180,15 @@
   </si>
   <si>
     <t>TTimer</t>
+  </si>
+  <si>
+    <t>TEdgeBox</t>
+  </si>
+  <si>
+    <t>TEdgeManager</t>
+  </si>
+  <si>
+    <t>TPlunger</t>
   </si>
 </sst>
 </file>
@@ -2741,8 +2750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A401" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E423" sqref="E423"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2762,19 +2771,19 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:297</v>
+        <v>Done:326</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
-        <v>Inp:3</v>
+        <v>Inp:2</v>
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.37678906368813264</v>
+        <v>0.42883455279744503</v>
       </c>
       <c r="E1" s="7" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:37</v>
+        <v>Classes:40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3699,13 +3708,17 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="15">
+      <c r="A72" s="19" t="s">
+        <v>715</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C72" s="19"/>
+      <c r="D72" s="20">
         <v>360</v>
       </c>
-      <c r="E72" s="6" t="s">
+      <c r="E72" s="21" t="s">
         <v>457</v>
       </c>
     </row>
@@ -4920,13 +4933,17 @@
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="2"/>
-      <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
-      <c r="D163" s="15">
+      <c r="A163" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="B163" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C163" s="19"/>
+      <c r="D163" s="20">
         <v>39</v>
       </c>
-      <c r="E163" s="6" t="s">
+      <c r="E163" s="21" t="s">
         <v>501</v>
       </c>
     </row>
@@ -6513,13 +6530,17 @@
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A276" s="2"/>
-      <c r="B276" s="2"/>
-      <c r="C276" s="2"/>
-      <c r="D276" s="15">
+      <c r="A276" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="B276" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C276" s="8"/>
+      <c r="D276" s="13">
         <v>387</v>
       </c>
-      <c r="E276" s="6" t="s">
+      <c r="E276" s="9" t="s">
         <v>121</v>
       </c>
     </row>
@@ -8218,7 +8239,9 @@
       <c r="A412" s="8" t="s">
         <v>706</v>
       </c>
-      <c r="B412" s="8"/>
+      <c r="B412" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C412" s="8"/>
       <c r="D412" s="13">
         <v>97</v>
@@ -8566,167 +8589,231 @@
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A439" s="2"/>
-      <c r="B439" s="2"/>
-      <c r="C439" s="2"/>
-      <c r="D439" s="15">
+      <c r="A439" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="B439" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C439" s="8" t="s">
+        <v>678</v>
+      </c>
+      <c r="D439" s="13">
         <v>78</v>
       </c>
-      <c r="E439" s="6" t="s">
+      <c r="E439" s="9" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A440" s="2"/>
-      <c r="B440" s="2"/>
-      <c r="C440" s="2"/>
-      <c r="D440" s="15">
+      <c r="A440" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="B440" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C440" s="8"/>
+      <c r="D440" s="13">
         <v>23</v>
       </c>
-      <c r="E440" s="6" t="s">
+      <c r="E440" s="9" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A441" s="2"/>
-      <c r="B441" s="2"/>
-      <c r="C441" s="2"/>
-      <c r="D441" s="15">
+      <c r="A441" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="B441" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C441" s="8"/>
+      <c r="D441" s="13">
         <v>30</v>
       </c>
-      <c r="E441" s="6" t="s">
+      <c r="E441" s="9" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A442" s="2"/>
-      <c r="B442" s="2"/>
-      <c r="C442" s="2"/>
-      <c r="D442" s="15">
+      <c r="A442" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B442" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C442" s="19" t="s">
+        <v>678</v>
+      </c>
+      <c r="D442" s="20">
         <v>33</v>
       </c>
-      <c r="E442" s="6" t="s">
+      <c r="E442" s="21" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A443" s="2"/>
-      <c r="B443" s="2"/>
-      <c r="C443" s="2"/>
-      <c r="D443" s="15">
+      <c r="A443" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B443" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C443" s="19"/>
+      <c r="D443" s="20">
         <v>15</v>
       </c>
-      <c r="E443" s="6" t="s">
+      <c r="E443" s="21" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A444" s="2"/>
-      <c r="B444" s="2"/>
-      <c r="C444" s="2"/>
-      <c r="D444" s="15">
+      <c r="A444" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B444" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C444" s="19"/>
+      <c r="D444" s="20">
         <v>35</v>
       </c>
-      <c r="E444" s="6" t="s">
+      <c r="E444" s="21" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A445" s="2"/>
-      <c r="B445" s="2"/>
-      <c r="C445" s="2"/>
-      <c r="D445" s="15">
+      <c r="A445" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B445" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C445" s="19"/>
+      <c r="D445" s="20">
         <v>37</v>
       </c>
-      <c r="E445" s="6" t="s">
+      <c r="E445" s="21" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A446" s="2"/>
-      <c r="B446" s="2"/>
-      <c r="C446" s="2"/>
-      <c r="D446" s="15">
+      <c r="A446" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B446" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C446" s="19"/>
+      <c r="D446" s="20">
         <v>181</v>
       </c>
-      <c r="E446" s="6" t="s">
+      <c r="E446" s="21" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A447" s="2"/>
-      <c r="B447" s="2"/>
-      <c r="C447" s="2"/>
-      <c r="D447" s="15">
+      <c r="A447" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B447" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C447" s="19"/>
+      <c r="D447" s="20">
         <v>181</v>
       </c>
-      <c r="E447" s="6" t="s">
+      <c r="E447" s="21" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A448" s="2"/>
-      <c r="B448" s="2"/>
-      <c r="C448" s="2"/>
-      <c r="D448" s="15">
+      <c r="A448" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B448" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C448" s="19"/>
+      <c r="D448" s="20">
         <v>147</v>
       </c>
-      <c r="E448" s="6" t="s">
+      <c r="E448" s="21" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A449" s="2"/>
-      <c r="B449" s="2"/>
-      <c r="C449" s="2"/>
-      <c r="D449" s="15">
+      <c r="A449" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B449" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C449" s="19"/>
+      <c r="D449" s="20">
         <v>1016</v>
       </c>
-      <c r="E449" s="6" t="s">
+      <c r="E449" s="21" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A450" s="2"/>
-      <c r="B450" s="2"/>
-      <c r="C450" s="2"/>
-      <c r="D450" s="15">
+      <c r="A450" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B450" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C450" s="19"/>
+      <c r="D450" s="20">
         <v>23</v>
       </c>
-      <c r="E450" s="6" t="s">
+      <c r="E450" s="21" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A451" s="2"/>
-      <c r="B451" s="2"/>
-      <c r="C451" s="2"/>
-      <c r="D451" s="15">
+      <c r="A451" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B451" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C451" s="19"/>
+      <c r="D451" s="20">
         <v>23</v>
       </c>
-      <c r="E451" s="6" t="s">
+      <c r="E451" s="21" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A452" s="2"/>
-      <c r="B452" s="2"/>
-      <c r="C452" s="2"/>
-      <c r="D452" s="15">
+      <c r="A452" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B452" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C452" s="19"/>
+      <c r="D452" s="20">
         <v>134</v>
       </c>
-      <c r="E452" s="6" t="s">
+      <c r="E452" s="21" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A453" s="2"/>
-      <c r="B453" s="2"/>
-      <c r="C453" s="2"/>
-      <c r="D453" s="15">
+      <c r="A453" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="B453" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C453" s="19"/>
+      <c r="D453" s="20">
         <v>211</v>
       </c>
-      <c r="E453" s="6" t="s">
+      <c r="E453" s="21" t="s">
         <v>234</v>
       </c>
     </row>
@@ -9636,7 +9723,9 @@
       <c r="A532" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="B532" s="8"/>
+      <c r="B532" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C532" s="8"/>
       <c r="D532" s="13">
         <v>40</v>
@@ -9679,7 +9768,9 @@
       <c r="A535" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="B535" s="8"/>
+      <c r="B535" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C535" s="8"/>
       <c r="D535" s="13">
         <v>764</v>
@@ -10065,7 +10156,7 @@
         <v>23</v>
       </c>
       <c r="B562" s="11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C562" s="11"/>
       <c r="D562" s="14">
@@ -10076,68 +10167,92 @@
       </c>
     </row>
     <row r="563" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A563" s="2"/>
-      <c r="B563" s="2"/>
-      <c r="C563" s="2"/>
-      <c r="D563" s="15">
+      <c r="A563" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="B563" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C563" s="8"/>
+      <c r="D563" s="13">
         <v>31</v>
       </c>
-      <c r="E563" s="6" t="s">
+      <c r="E563" s="9" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A564" s="2"/>
-      <c r="B564" s="2"/>
-      <c r="C564" s="2"/>
-      <c r="D564" s="15">
+      <c r="A564" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="B564" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C564" s="8"/>
+      <c r="D564" s="13">
         <v>114</v>
       </c>
-      <c r="E564" s="6" t="s">
+      <c r="E564" s="9" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A565" s="2"/>
-      <c r="B565" s="2"/>
-      <c r="C565" s="2"/>
-      <c r="D565" s="15">
+      <c r="A565" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="B565" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C565" s="8"/>
+      <c r="D565" s="13">
         <v>380</v>
       </c>
-      <c r="E565" s="6" t="s">
+      <c r="E565" s="9" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A566" s="2"/>
-      <c r="B566" s="2"/>
-      <c r="C566" s="2"/>
-      <c r="D566" s="15">
+      <c r="A566" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="B566" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C566" s="8"/>
+      <c r="D566" s="13">
         <v>26</v>
       </c>
-      <c r="E566" s="6" t="s">
+      <c r="E566" s="9" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="567" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A567" s="2"/>
-      <c r="B567" s="2"/>
-      <c r="C567" s="2"/>
-      <c r="D567" s="15">
+      <c r="A567" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="B567" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C567" s="8"/>
+      <c r="D567" s="13">
         <v>175</v>
       </c>
-      <c r="E567" s="6" t="s">
+      <c r="E567" s="9" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A568" s="2"/>
-      <c r="B568" s="2"/>
-      <c r="C568" s="2"/>
-      <c r="D568" s="15">
+      <c r="A568" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="B568" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C568" s="8"/>
+      <c r="D568" s="13">
         <v>179</v>
       </c>
-      <c r="E568" s="6" t="s">
+      <c r="E568" s="9" t="s">
         <v>349</v>
       </c>
     </row>
@@ -10590,7 +10705,9 @@
       <c r="A606" s="16" t="s">
         <v>715</v>
       </c>
-      <c r="B606" s="16"/>
+      <c r="B606" s="16" t="s">
+        <v>668</v>
+      </c>
       <c r="C606" s="16"/>
       <c r="D606" s="17">
         <v>85</v>

</xml_diff>

<commit_message>
TRollover, TOneway, TLightRollover, TTripwire, TEdgeManager ready.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="730">
   <si>
     <t>Function</t>
   </si>
@@ -2189,6 +2189,21 @@
   </si>
   <si>
     <t>TPlunger</t>
+  </si>
+  <si>
+    <t>TLighRollover</t>
+  </si>
+  <si>
+    <t>TLighGroup</t>
+  </si>
+  <si>
+    <t>TOneway</t>
+  </si>
+  <si>
+    <t>TRollover</t>
+  </si>
+  <si>
+    <t>TTripwire</t>
   </si>
 </sst>
 </file>
@@ -2325,7 +2340,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2377,6 +2392,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2751,7 +2769,7 @@
   <dimension ref="A1:E669"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2771,7 +2789,7 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:326</v>
+        <v>Done:361</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
@@ -2779,11 +2797,11 @@
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.42883455279744503</v>
-      </c>
-      <c r="E1" s="7" t="str">
+        <v>0.47723854745771305</v>
+      </c>
+      <c r="E1" s="25" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:40</v>
+        <v>Classes:44.9999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3555,24 +3573,32 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="15">
+      <c r="A59" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C59" s="8"/>
+      <c r="D59" s="13">
         <v>255</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E59" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="15">
+      <c r="A60" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="13">
         <v>33</v>
       </c>
-      <c r="E60" s="6" t="s">
+      <c r="E60" s="9" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3631,24 +3657,30 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="15">
+      <c r="A65" s="19" t="s">
+        <v>700</v>
+      </c>
+      <c r="B65" s="19"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="20">
         <v>41</v>
       </c>
-      <c r="E65" s="6" t="s">
+      <c r="E65" s="21" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="15">
+      <c r="A66" s="19" t="s">
+        <v>700</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C66" s="19"/>
+      <c r="D66" s="20">
         <v>35</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="E66" s="21" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3697,13 +3729,17 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="15">
+      <c r="A71" s="19" t="s">
+        <v>715</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C71" s="19"/>
+      <c r="D71" s="20">
         <v>1109</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E71" s="21" t="s">
         <v>456</v>
       </c>
     </row>
@@ -8269,7 +8305,9 @@
       <c r="A414" s="8" t="s">
         <v>706</v>
       </c>
-      <c r="B414" s="8"/>
+      <c r="B414" s="8" t="s">
+        <v>668</v>
+      </c>
       <c r="C414" s="8"/>
       <c r="D414" s="13">
         <v>13</v>
@@ -9555,167 +9593,227 @@
       </c>
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A517" s="2"/>
-      <c r="B517" s="2"/>
-      <c r="C517" s="2"/>
-      <c r="D517" s="15">
+      <c r="A517" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B517" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C517" s="8"/>
+      <c r="D517" s="13">
         <v>33</v>
       </c>
-      <c r="E517" s="6" t="s">
+      <c r="E517" s="9" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A518" s="2"/>
-      <c r="B518" s="2"/>
-      <c r="C518" s="2"/>
-      <c r="D518" s="15">
+      <c r="A518" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B518" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C518" s="8"/>
+      <c r="D518" s="13">
         <v>21</v>
       </c>
-      <c r="E518" s="6" t="s">
+      <c r="E518" s="9" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A519" s="2"/>
-      <c r="B519" s="2"/>
-      <c r="C519" s="2"/>
-      <c r="D519" s="15">
+      <c r="A519" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B519" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C519" s="8"/>
+      <c r="D519" s="13">
         <v>2234</v>
       </c>
-      <c r="E519" s="6" t="s">
+      <c r="E519" s="9" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A520" s="2"/>
-      <c r="B520" s="2"/>
-      <c r="C520" s="2"/>
-      <c r="D520" s="15">
+      <c r="A520" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B520" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C520" s="8"/>
+      <c r="D520" s="13">
         <v>33</v>
       </c>
-      <c r="E520" s="6" t="s">
+      <c r="E520" s="9" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A521" s="2"/>
-      <c r="B521" s="2"/>
-      <c r="C521" s="2"/>
-      <c r="D521" s="15">
+      <c r="A521" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B521" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C521" s="8"/>
+      <c r="D521" s="13">
         <v>37</v>
       </c>
-      <c r="E521" s="6" t="s">
+      <c r="E521" s="9" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A522" s="2"/>
-      <c r="B522" s="2"/>
-      <c r="C522" s="2"/>
-      <c r="D522" s="15">
+      <c r="A522" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B522" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C522" s="8"/>
+      <c r="D522" s="13">
         <v>24</v>
       </c>
-      <c r="E522" s="6" t="s">
+      <c r="E522" s="9" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A523" s="2"/>
-      <c r="B523" s="2"/>
-      <c r="C523" s="2"/>
-      <c r="D523" s="15">
+      <c r="A523" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B523" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C523" s="8"/>
+      <c r="D523" s="13">
         <v>101</v>
       </c>
-      <c r="E523" s="6" t="s">
+      <c r="E523" s="9" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A524" s="2"/>
-      <c r="B524" s="2"/>
-      <c r="C524" s="2"/>
-      <c r="D524" s="15">
+      <c r="A524" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B524" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C524" s="8"/>
+      <c r="D524" s="13">
         <v>55</v>
       </c>
-      <c r="E524" s="6" t="s">
+      <c r="E524" s="9" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A525" s="2"/>
-      <c r="B525" s="2"/>
-      <c r="C525" s="2"/>
-      <c r="D525" s="15">
+      <c r="A525" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B525" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C525" s="8"/>
+      <c r="D525" s="13">
         <v>64</v>
       </c>
-      <c r="E525" s="6" t="s">
+      <c r="E525" s="9" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A526" s="2"/>
-      <c r="B526" s="2"/>
-      <c r="C526" s="2"/>
-      <c r="D526" s="15">
+      <c r="A526" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B526" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C526" s="8"/>
+      <c r="D526" s="13">
         <v>30</v>
       </c>
-      <c r="E526" s="6" t="s">
+      <c r="E526" s="9" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A527" s="2"/>
-      <c r="B527" s="2"/>
-      <c r="C527" s="2"/>
-      <c r="D527" s="15">
+      <c r="A527" s="8" t="s">
+        <v>726</v>
+      </c>
+      <c r="B527" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C527" s="8"/>
+      <c r="D527" s="13">
         <v>150</v>
       </c>
-      <c r="E527" s="6" t="s">
+      <c r="E527" s="9" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A528" s="2"/>
-      <c r="B528" s="2"/>
-      <c r="C528" s="2"/>
-      <c r="D528" s="15">
+      <c r="A528" s="19" t="s">
+        <v>725</v>
+      </c>
+      <c r="B528" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C528" s="19"/>
+      <c r="D528" s="20">
         <v>176</v>
       </c>
-      <c r="E528" s="6" t="s">
+      <c r="E528" s="21" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A529" s="2"/>
-      <c r="B529" s="2"/>
-      <c r="C529" s="2"/>
-      <c r="D529" s="15">
+      <c r="A529" s="19" t="s">
+        <v>725</v>
+      </c>
+      <c r="B529" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C529" s="19"/>
+      <c r="D529" s="20">
         <v>28</v>
       </c>
-      <c r="E529" s="6" t="s">
+      <c r="E529" s="21" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A530" s="2"/>
-      <c r="B530" s="2"/>
-      <c r="C530" s="2"/>
-      <c r="D530" s="15">
+      <c r="A530" s="19" t="s">
+        <v>725</v>
+      </c>
+      <c r="B530" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C530" s="19"/>
+      <c r="D530" s="20">
         <v>65</v>
       </c>
-      <c r="E530" s="6" t="s">
+      <c r="E530" s="21" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A531" s="2"/>
-      <c r="B531" s="2"/>
-      <c r="C531" s="2"/>
-      <c r="D531" s="15">
+      <c r="A531" s="19" t="s">
+        <v>725</v>
+      </c>
+      <c r="B531" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C531" s="19"/>
+      <c r="D531" s="20">
         <v>86</v>
       </c>
-      <c r="E531" s="6" t="s">
+      <c r="E531" s="21" t="s">
         <v>311</v>
       </c>
     </row>
@@ -9810,57 +9908,77 @@
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A538" s="2"/>
-      <c r="B538" s="2"/>
-      <c r="C538" s="2"/>
-      <c r="D538" s="15">
+      <c r="A538" s="19" t="s">
+        <v>727</v>
+      </c>
+      <c r="B538" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C538" s="19"/>
+      <c r="D538" s="20">
         <v>33</v>
       </c>
-      <c r="E538" s="6" t="s">
+      <c r="E538" s="21" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A539" s="2"/>
-      <c r="B539" s="2"/>
-      <c r="C539" s="2"/>
-      <c r="D539" s="15">
+      <c r="A539" s="19" t="s">
+        <v>727</v>
+      </c>
+      <c r="B539" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C539" s="19"/>
+      <c r="D539" s="20">
         <v>230</v>
       </c>
-      <c r="E539" s="6" t="s">
+      <c r="E539" s="21" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A540" s="2"/>
-      <c r="B540" s="2"/>
-      <c r="C540" s="2"/>
-      <c r="D540" s="15">
+      <c r="A540" s="19" t="s">
+        <v>727</v>
+      </c>
+      <c r="B540" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C540" s="19"/>
+      <c r="D540" s="20">
         <v>25</v>
       </c>
-      <c r="E540" s="6" t="s">
+      <c r="E540" s="21" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A541" s="2"/>
-      <c r="B541" s="2"/>
-      <c r="C541" s="2"/>
-      <c r="D541" s="15">
+      <c r="A541" s="19" t="s">
+        <v>727</v>
+      </c>
+      <c r="B541" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C541" s="19"/>
+      <c r="D541" s="20">
         <v>24</v>
       </c>
-      <c r="E541" s="6" t="s">
+      <c r="E541" s="21" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A542" s="2"/>
-      <c r="B542" s="2"/>
-      <c r="C542" s="2"/>
-      <c r="D542" s="15">
+      <c r="A542" s="19" t="s">
+        <v>727</v>
+      </c>
+      <c r="B542" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C542" s="19"/>
+      <c r="D542" s="20">
         <v>256</v>
       </c>
-      <c r="E542" s="6" t="s">
+      <c r="E542" s="21" t="s">
         <v>320</v>
       </c>
     </row>
@@ -10403,90 +10521,122 @@
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A581" s="2"/>
-      <c r="B581" s="2"/>
-      <c r="C581" s="2"/>
-      <c r="D581" s="15">
+      <c r="A581" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="B581" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C581" s="19"/>
+      <c r="D581" s="20">
         <v>104</v>
       </c>
-      <c r="E581" s="6" t="s">
+      <c r="E581" s="21" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A582" s="2"/>
-      <c r="B582" s="2"/>
-      <c r="C582" s="2"/>
-      <c r="D582" s="15">
+      <c r="A582" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="B582" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C582" s="19"/>
+      <c r="D582" s="20">
         <v>146</v>
       </c>
-      <c r="E582" s="6" t="s">
+      <c r="E582" s="21" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A583" s="2"/>
-      <c r="B583" s="2"/>
-      <c r="C583" s="2"/>
-      <c r="D583" s="15">
+      <c r="A583" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="B583" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C583" s="19"/>
+      <c r="D583" s="20">
         <v>25</v>
       </c>
-      <c r="E583" s="6" t="s">
+      <c r="E583" s="21" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A584" s="2"/>
-      <c r="B584" s="2"/>
-      <c r="C584" s="2"/>
-      <c r="D584" s="15">
+      <c r="A584" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="B584" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C584" s="19"/>
+      <c r="D584" s="20">
         <v>49</v>
       </c>
-      <c r="E584" s="6" t="s">
+      <c r="E584" s="21" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A585" s="2"/>
-      <c r="B585" s="2"/>
-      <c r="C585" s="2"/>
-      <c r="D585" s="15">
+      <c r="A585" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="B585" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C585" s="19"/>
+      <c r="D585" s="20">
         <v>24</v>
       </c>
-      <c r="E585" s="6" t="s">
+      <c r="E585" s="21" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A586" s="2"/>
-      <c r="B586" s="2"/>
-      <c r="C586" s="2"/>
-      <c r="D586" s="15">
+      <c r="A586" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="B586" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C586" s="19"/>
+      <c r="D586" s="20">
         <v>16</v>
       </c>
-      <c r="E586" s="6" t="s">
+      <c r="E586" s="21" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="587" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A587" s="2"/>
-      <c r="B587" s="2"/>
-      <c r="C587" s="2"/>
-      <c r="D587" s="15">
+      <c r="A587" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="B587" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C587" s="19"/>
+      <c r="D587" s="20">
         <v>69</v>
       </c>
-      <c r="E587" s="6" t="s">
+      <c r="E587" s="21" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A588" s="2"/>
-      <c r="B588" s="2"/>
-      <c r="C588" s="2"/>
-      <c r="D588" s="15">
+      <c r="A588" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="B588" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C588" s="19"/>
+      <c r="D588" s="20">
         <v>35</v>
       </c>
-      <c r="E588" s="6" t="s">
+      <c r="E588" s="21" t="s">
         <v>365</v>
       </c>
     </row>
@@ -10957,24 +11107,32 @@
       </c>
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A623" s="2"/>
-      <c r="B623" s="2"/>
-      <c r="C623" s="2"/>
-      <c r="D623" s="15">
+      <c r="A623" s="19" t="s">
+        <v>729</v>
+      </c>
+      <c r="B623" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C623" s="19"/>
+      <c r="D623" s="20">
         <v>77</v>
       </c>
-      <c r="E623" s="6" t="s">
+      <c r="E623" s="21" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A624" s="2"/>
-      <c r="B624" s="2"/>
-      <c r="C624" s="2"/>
-      <c r="D624" s="15">
+      <c r="A624" s="19" t="s">
+        <v>729</v>
+      </c>
+      <c r="B624" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C624" s="19"/>
+      <c r="D624" s="20">
         <v>34</v>
       </c>
-      <c r="E624" s="6" t="s">
+      <c r="E624" s="21" t="s">
         <v>405</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TBlocker, TBumper, TFlagSpinner, TGate, THole, TKickback, TWall ready.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1495" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="739">
   <si>
     <t>Function</t>
   </si>
@@ -2167,9 +2167,6 @@
     <t>nudge</t>
   </si>
   <si>
-    <t>Tball</t>
-  </si>
-  <si>
     <t>TComponentGroup</t>
   </si>
   <si>
@@ -2210,6 +2207,30 @@
   </si>
   <si>
     <t>TFlipper</t>
+  </si>
+  <si>
+    <t>TBlocker</t>
+  </si>
+  <si>
+    <t>TBall</t>
+  </si>
+  <si>
+    <t>TBumper</t>
+  </si>
+  <si>
+    <t>TFlagSpinner</t>
+  </si>
+  <si>
+    <t>TGate</t>
+  </si>
+  <si>
+    <t>THole</t>
+  </si>
+  <si>
+    <t>TKickback</t>
+  </si>
+  <si>
+    <t>TWall</t>
   </si>
 </sst>
 </file>
@@ -2795,7 +2816,7 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:383</v>
+        <v>Done:417</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
@@ -2803,11 +2824,11 @@
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.52307406343466434</v>
+        <v>0.55391270552053939</v>
       </c>
       <c r="E1" s="25" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:46.9999999999999</v>
+        <v>Classes:53.9999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3859,7 +3880,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>668</v>
@@ -3874,7 +3895,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>668</v>
@@ -3889,7 +3910,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B82" s="8" t="s">
         <v>668</v>
@@ -8108,7 +8129,7 @@
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A397" s="8" t="s">
-        <v>717</v>
+        <v>732</v>
       </c>
       <c r="B397" s="8" t="s">
         <v>668</v>
@@ -8123,7 +8144,7 @@
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A398" s="8" t="s">
-        <v>717</v>
+        <v>732</v>
       </c>
       <c r="B398" s="8" t="s">
         <v>668</v>
@@ -8138,7 +8159,7 @@
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A399" s="8" t="s">
-        <v>717</v>
+        <v>732</v>
       </c>
       <c r="B399" s="8" t="s">
         <v>668</v>
@@ -8153,7 +8174,7 @@
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A400" s="8" t="s">
-        <v>717</v>
+        <v>732</v>
       </c>
       <c r="B400" s="8" t="s">
         <v>668</v>
@@ -8168,7 +8189,7 @@
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" s="8" t="s">
-        <v>717</v>
+        <v>732</v>
       </c>
       <c r="B401" s="8" t="s">
         <v>668</v>
@@ -8182,112 +8203,152 @@
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A402" s="2"/>
-      <c r="B402" s="2"/>
-      <c r="C402" s="2"/>
-      <c r="D402" s="15">
+      <c r="A402" s="19" t="s">
+        <v>731</v>
+      </c>
+      <c r="B402" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C402" s="19"/>
+      <c r="D402" s="20">
         <v>186</v>
       </c>
-      <c r="E402" s="6" t="s">
+      <c r="E402" s="21" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A403" s="2"/>
-      <c r="B403" s="2"/>
-      <c r="C403" s="2"/>
-      <c r="D403" s="15">
+      <c r="A403" s="19" t="s">
+        <v>731</v>
+      </c>
+      <c r="B403" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C403" s="19"/>
+      <c r="D403" s="20">
         <v>105</v>
       </c>
-      <c r="E403" s="6" t="s">
+      <c r="E403" s="21" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A404" s="2"/>
-      <c r="B404" s="2"/>
-      <c r="C404" s="2"/>
-      <c r="D404" s="15">
+      <c r="A404" s="19" t="s">
+        <v>731</v>
+      </c>
+      <c r="B404" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C404" s="19"/>
+      <c r="D404" s="20">
         <v>24</v>
       </c>
-      <c r="E404" s="6" t="s">
+      <c r="E404" s="21" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A405" s="2"/>
-      <c r="B405" s="2"/>
-      <c r="C405" s="2"/>
-      <c r="D405" s="15">
+      <c r="A405" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="B405" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C405" s="16"/>
+      <c r="D405" s="17">
         <v>46</v>
       </c>
-      <c r="E405" s="6" t="s">
+      <c r="E405" s="18" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A406" s="2"/>
-      <c r="B406" s="2"/>
-      <c r="C406" s="2"/>
-      <c r="D406" s="15">
+      <c r="A406" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="B406" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C406" s="16"/>
+      <c r="D406" s="17">
         <v>101</v>
       </c>
-      <c r="E406" s="6" t="s">
+      <c r="E406" s="18" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A407" s="2"/>
-      <c r="B407" s="2"/>
-      <c r="C407" s="2"/>
-      <c r="D407" s="15">
+      <c r="A407" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="B407" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C407" s="16"/>
+      <c r="D407" s="17">
         <v>25</v>
       </c>
-      <c r="E407" s="6" t="s">
+      <c r="E407" s="18" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A408" s="2"/>
-      <c r="B408" s="2"/>
-      <c r="C408" s="2"/>
-      <c r="D408" s="15">
+      <c r="A408" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="B408" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C408" s="16"/>
+      <c r="D408" s="17">
         <v>379</v>
       </c>
-      <c r="E408" s="6" t="s">
+      <c r="E408" s="18" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A409" s="2"/>
-      <c r="B409" s="2"/>
-      <c r="C409" s="2"/>
-      <c r="D409" s="15">
+      <c r="A409" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="B409" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C409" s="16"/>
+      <c r="D409" s="17">
         <v>24</v>
       </c>
-      <c r="E409" s="6" t="s">
+      <c r="E409" s="18" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A410" s="2"/>
-      <c r="B410" s="2"/>
-      <c r="C410" s="2"/>
-      <c r="D410" s="15">
+      <c r="A410" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="B410" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C410" s="16"/>
+      <c r="D410" s="17">
         <v>97</v>
       </c>
-      <c r="E410" s="6" t="s">
+      <c r="E410" s="18" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A411" s="2"/>
-      <c r="B411" s="2"/>
-      <c r="C411" s="2"/>
-      <c r="D411" s="15">
+      <c r="A411" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="B411" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C411" s="16"/>
+      <c r="D411" s="17">
         <v>88</v>
       </c>
-      <c r="E411" s="6" t="s">
+      <c r="E411" s="18" t="s">
         <v>198</v>
       </c>
     </row>
@@ -8428,7 +8489,7 @@
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" s="8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B421" s="8" t="s">
         <v>668</v>
@@ -8445,7 +8506,7 @@
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422" s="8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B422" s="8" t="s">
         <v>668</v>
@@ -8460,7 +8521,7 @@
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423" s="8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B423" s="8" t="s">
         <v>668</v>
@@ -8475,7 +8536,7 @@
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A424" s="8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B424" s="8" t="s">
         <v>668</v>
@@ -8490,7 +8551,7 @@
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" s="8" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B425" s="8" t="s">
         <v>668</v>
@@ -8648,7 +8709,7 @@
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A439" s="8" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B439" s="8" t="s">
         <v>668</v>
@@ -8665,7 +8726,7 @@
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A440" s="8" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B440" s="8" t="s">
         <v>668</v>
@@ -8680,7 +8741,7 @@
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" s="8" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B441" s="8" t="s">
         <v>668</v>
@@ -8695,7 +8756,7 @@
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A442" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B442" s="19" t="s">
         <v>668</v>
@@ -8712,7 +8773,7 @@
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A443" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B443" s="19" t="s">
         <v>668</v>
@@ -8727,7 +8788,7 @@
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B444" s="19" t="s">
         <v>668</v>
@@ -8742,7 +8803,7 @@
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A445" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B445" s="19" t="s">
         <v>668</v>
@@ -8757,7 +8818,7 @@
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A446" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B446" s="19" t="s">
         <v>668</v>
@@ -8772,7 +8833,7 @@
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A447" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B447" s="19" t="s">
         <v>668</v>
@@ -8787,7 +8848,7 @@
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A448" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B448" s="19" t="s">
         <v>668</v>
@@ -8802,7 +8863,7 @@
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A449" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B449" s="19" t="s">
         <v>668</v>
@@ -8817,7 +8878,7 @@
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A450" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B450" s="19" t="s">
         <v>668</v>
@@ -8832,7 +8893,7 @@
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A451" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B451" s="19" t="s">
         <v>668</v>
@@ -8847,7 +8908,7 @@
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A452" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B452" s="19" t="s">
         <v>668</v>
@@ -8862,7 +8923,7 @@
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A453" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B453" s="19" t="s">
         <v>668</v>
@@ -8891,85 +8952,113 @@
       </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A455" s="2"/>
-      <c r="B455" s="2"/>
-      <c r="C455" s="2"/>
-      <c r="D455" s="15">
+      <c r="A455" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="B455" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C455" s="16"/>
+      <c r="D455" s="17">
         <v>152</v>
       </c>
-      <c r="E455" s="6" t="s">
+      <c r="E455" s="18" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A456" s="2"/>
-      <c r="B456" s="2"/>
-      <c r="C456" s="2"/>
-      <c r="D456" s="15">
+      <c r="A456" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="B456" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C456" s="16"/>
+      <c r="D456" s="17">
         <v>25</v>
       </c>
-      <c r="E456" s="6" t="s">
+      <c r="E456" s="18" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A457" s="2"/>
-      <c r="B457" s="2"/>
-      <c r="C457" s="2"/>
-      <c r="D457" s="15">
+      <c r="A457" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="B457" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C457" s="16"/>
+      <c r="D457" s="17">
         <v>95</v>
       </c>
-      <c r="E457" s="6" t="s">
+      <c r="E457" s="18" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A458" s="2"/>
-      <c r="B458" s="2"/>
-      <c r="C458" s="2"/>
-      <c r="D458" s="15">
+      <c r="A458" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="B458" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C458" s="16"/>
+      <c r="D458" s="17">
         <v>193</v>
       </c>
-      <c r="E458" s="6" t="s">
+      <c r="E458" s="18" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A459" s="2"/>
-      <c r="B459" s="2"/>
-      <c r="C459" s="2"/>
-      <c r="D459" s="15">
+      <c r="A459" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="B459" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C459" s="16"/>
+      <c r="D459" s="17">
         <v>24</v>
       </c>
-      <c r="E459" s="6" t="s">
+      <c r="E459" s="18" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A460" s="2"/>
-      <c r="B460" s="2"/>
-      <c r="C460" s="2"/>
-      <c r="D460" s="15">
+      <c r="A460" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="B460" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C460" s="16"/>
+      <c r="D460" s="17">
         <v>21</v>
       </c>
-      <c r="E460" s="6" t="s">
+      <c r="E460" s="18" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A461" s="2"/>
-      <c r="B461" s="2"/>
-      <c r="C461" s="2"/>
-      <c r="D461" s="15">
+      <c r="A461" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="B461" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C461" s="16"/>
+      <c r="D461" s="17">
         <v>299</v>
       </c>
-      <c r="E461" s="6" t="s">
+      <c r="E461" s="18" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A462" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B462" s="19" t="s">
         <v>668</v>
@@ -8984,7 +9073,7 @@
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A463" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B463" s="19" t="s">
         <v>668</v>
@@ -8999,7 +9088,7 @@
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B464" s="19" t="s">
         <v>668</v>
@@ -9014,7 +9103,7 @@
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A465" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B465" s="19" t="s">
         <v>668</v>
@@ -9029,7 +9118,7 @@
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A466" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B466" s="19" t="s">
         <v>668</v>
@@ -9044,7 +9133,7 @@
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A467" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B467" s="19" t="s">
         <v>668</v>
@@ -9059,7 +9148,7 @@
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A468" s="19" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B468" s="19" t="s">
         <v>668</v>
@@ -9074,7 +9163,7 @@
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A469" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B469" s="8" t="s">
         <v>668</v>
@@ -9089,7 +9178,7 @@
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A470" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B470" s="8" t="s">
         <v>668</v>
@@ -9104,7 +9193,7 @@
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A471" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B471" s="8" t="s">
         <v>668</v>
@@ -9119,7 +9208,7 @@
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A472" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B472" s="8" t="s">
         <v>668</v>
@@ -9134,7 +9223,7 @@
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A473" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B473" s="8" t="s">
         <v>668</v>
@@ -9149,7 +9238,7 @@
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A474" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B474" s="8" t="s">
         <v>668</v>
@@ -9164,7 +9253,7 @@
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A475" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B475" s="8" t="s">
         <v>668</v>
@@ -9179,7 +9268,7 @@
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A476" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B476" s="8" t="s">
         <v>668</v>
@@ -9194,7 +9283,7 @@
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A477" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B477" s="8" t="s">
         <v>668</v>
@@ -9209,7 +9298,7 @@
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A478" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B478" s="8" t="s">
         <v>668</v>
@@ -9223,79 +9312,107 @@
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A479" s="2"/>
-      <c r="B479" s="2"/>
-      <c r="C479" s="2"/>
-      <c r="D479" s="15">
+      <c r="A479" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="B479" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C479" s="19"/>
+      <c r="D479" s="20">
         <v>107</v>
       </c>
-      <c r="E479" s="6" t="s">
+      <c r="E479" s="21" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A480" s="2"/>
-      <c r="B480" s="2"/>
-      <c r="C480" s="2"/>
-      <c r="D480" s="15">
+      <c r="A480" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="B480" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C480" s="19"/>
+      <c r="D480" s="20">
         <v>95</v>
       </c>
-      <c r="E480" s="6" t="s">
+      <c r="E480" s="21" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A481" s="2"/>
-      <c r="B481" s="2"/>
-      <c r="C481" s="2"/>
-      <c r="D481" s="15">
+      <c r="A481" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="B481" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C481" s="8"/>
+      <c r="D481" s="13">
         <v>114</v>
       </c>
-      <c r="E481" s="6" t="s">
+      <c r="E481" s="9" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A482" s="2"/>
-      <c r="B482" s="2"/>
-      <c r="C482" s="2"/>
-      <c r="D482" s="15">
+      <c r="A482" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="B482" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C482" s="8"/>
+      <c r="D482" s="13">
         <v>236</v>
       </c>
-      <c r="E482" s="6" t="s">
+      <c r="E482" s="9" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A483" s="2"/>
-      <c r="B483" s="2"/>
-      <c r="C483" s="2"/>
-      <c r="D483" s="15">
+      <c r="A483" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="B483" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C483" s="8"/>
+      <c r="D483" s="13">
         <v>54</v>
       </c>
-      <c r="E483" s="6" t="s">
+      <c r="E483" s="9" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A484" s="2"/>
-      <c r="B484" s="2"/>
-      <c r="C484" s="2"/>
-      <c r="D484" s="15">
+      <c r="A484" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="B484" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C484" s="8"/>
+      <c r="D484" s="13">
         <v>407</v>
       </c>
-      <c r="E484" s="6" t="s">
+      <c r="E484" s="9" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A485" s="2"/>
-      <c r="B485" s="2"/>
-      <c r="C485" s="2"/>
-      <c r="D485" s="15">
+      <c r="A485" s="8" t="s">
+        <v>736</v>
+      </c>
+      <c r="B485" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C485" s="8"/>
+      <c r="D485" s="13">
         <v>23</v>
       </c>
-      <c r="E485" s="6" t="s">
+      <c r="E485" s="9" t="s">
         <v>274</v>
       </c>
     </row>
@@ -9408,46 +9525,62 @@
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A494" s="2"/>
-      <c r="B494" s="2"/>
-      <c r="C494" s="2"/>
-      <c r="D494" s="15">
+      <c r="A494" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="B494" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C494" s="8"/>
+      <c r="D494" s="13">
         <v>137</v>
       </c>
-      <c r="E494" s="6" t="s">
+      <c r="E494" s="9" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A495" s="2"/>
-      <c r="B495" s="2"/>
-      <c r="C495" s="2"/>
-      <c r="D495" s="15">
+      <c r="A495" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="B495" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C495" s="8"/>
+      <c r="D495" s="13">
         <v>74</v>
       </c>
-      <c r="E495" s="6" t="s">
+      <c r="E495" s="9" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A496" s="2"/>
-      <c r="B496" s="2"/>
-      <c r="C496" s="2"/>
-      <c r="D496" s="15">
+      <c r="A496" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="B496" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C496" s="8"/>
+      <c r="D496" s="13">
         <v>178</v>
       </c>
-      <c r="E496" s="6" t="s">
+      <c r="E496" s="9" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A497" s="2"/>
-      <c r="B497" s="2"/>
-      <c r="C497" s="2"/>
-      <c r="D497" s="15">
+      <c r="A497" s="8" t="s">
+        <v>737</v>
+      </c>
+      <c r="B497" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C497" s="8"/>
+      <c r="D497" s="13">
         <v>66</v>
       </c>
-      <c r="E497" s="6" t="s">
+      <c r="E497" s="9" t="s">
         <v>277</v>
       </c>
     </row>
@@ -9541,7 +9674,7 @@
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A506" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B506" s="8" t="s">
         <v>668</v>
@@ -9556,7 +9689,7 @@
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A507" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B507" s="8" t="s">
         <v>668</v>
@@ -9571,7 +9704,7 @@
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A508" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B508" s="8" t="s">
         <v>668</v>
@@ -9586,7 +9719,7 @@
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A509" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B509" s="8" t="s">
         <v>668</v>
@@ -9601,7 +9734,7 @@
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A510" s="8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B510" s="8" t="s">
         <v>668</v>
@@ -9682,7 +9815,7 @@
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A517" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B517" s="8" t="s">
         <v>668</v>
@@ -9697,7 +9830,7 @@
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A518" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B518" s="8" t="s">
         <v>668</v>
@@ -9712,7 +9845,7 @@
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A519" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B519" s="8" t="s">
         <v>668</v>
@@ -9727,7 +9860,7 @@
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A520" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B520" s="8" t="s">
         <v>668</v>
@@ -9742,7 +9875,7 @@
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A521" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B521" s="8" t="s">
         <v>668</v>
@@ -9757,7 +9890,7 @@
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A522" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B522" s="8" t="s">
         <v>668</v>
@@ -9772,7 +9905,7 @@
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A523" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B523" s="8" t="s">
         <v>668</v>
@@ -9787,7 +9920,7 @@
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A524" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B524" s="8" t="s">
         <v>668</v>
@@ -9802,7 +9935,7 @@
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A525" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B525" s="8" t="s">
         <v>668</v>
@@ -9817,7 +9950,7 @@
     </row>
     <row r="526" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A526" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B526" s="8" t="s">
         <v>668</v>
@@ -9832,7 +9965,7 @@
     </row>
     <row r="527" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A527" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B527" s="8" t="s">
         <v>668</v>
@@ -9847,7 +9980,7 @@
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A528" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B528" s="19" t="s">
         <v>668</v>
@@ -9862,7 +9995,7 @@
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A529" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B529" s="19" t="s">
         <v>668</v>
@@ -9877,7 +10010,7 @@
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A530" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B530" s="19" t="s">
         <v>668</v>
@@ -9892,7 +10025,7 @@
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A531" s="19" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B531" s="19" t="s">
         <v>668</v>
@@ -9997,7 +10130,7 @@
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A538" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B538" s="19" t="s">
         <v>668</v>
@@ -10012,7 +10145,7 @@
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A539" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B539" s="19" t="s">
         <v>668</v>
@@ -10027,7 +10160,7 @@
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A540" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B540" s="19" t="s">
         <v>668</v>
@@ -10042,7 +10175,7 @@
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A541" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B541" s="19" t="s">
         <v>668</v>
@@ -10057,7 +10190,7 @@
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A542" s="19" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B542" s="19" t="s">
         <v>668</v>
@@ -10374,7 +10507,7 @@
     </row>
     <row r="563" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A563" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B563" s="8" t="s">
         <v>668</v>
@@ -10389,7 +10522,7 @@
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A564" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B564" s="8" t="s">
         <v>668</v>
@@ -10404,7 +10537,7 @@
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A565" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B565" s="8" t="s">
         <v>668</v>
@@ -10419,7 +10552,7 @@
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A566" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B566" s="8" t="s">
         <v>668</v>
@@ -10434,7 +10567,7 @@
     </row>
     <row r="567" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A567" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B567" s="8" t="s">
         <v>668</v>
@@ -10449,7 +10582,7 @@
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A568" s="8" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B568" s="8" t="s">
         <v>668</v>
@@ -10610,7 +10743,7 @@
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A581" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B581" s="19" t="s">
         <v>668</v>
@@ -10625,7 +10758,7 @@
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A582" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B582" s="19" t="s">
         <v>668</v>
@@ -10640,7 +10773,7 @@
     </row>
     <row r="583" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A583" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B583" s="19" t="s">
         <v>668</v>
@@ -10655,7 +10788,7 @@
     </row>
     <row r="584" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A584" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B584" s="19" t="s">
         <v>668</v>
@@ -10670,7 +10803,7 @@
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A585" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B585" s="19" t="s">
         <v>668</v>
@@ -10685,7 +10818,7 @@
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A586" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B586" s="19" t="s">
         <v>668</v>
@@ -10700,7 +10833,7 @@
     </row>
     <row r="587" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A587" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B587" s="19" t="s">
         <v>668</v>
@@ -10715,7 +10848,7 @@
     </row>
     <row r="588" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A588" s="19" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B588" s="19" t="s">
         <v>668</v>
@@ -10862,7 +10995,7 @@
     </row>
     <row r="601" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A601" s="8" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B601" s="8" t="s">
         <v>668</v>
@@ -10879,7 +11012,7 @@
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A602" s="8" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B602" s="8" t="s">
         <v>668</v>
@@ -10894,7 +11027,7 @@
     </row>
     <row r="603" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A603" s="8" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B603" s="8" t="s">
         <v>668</v>
@@ -11151,7 +11284,7 @@
     </row>
     <row r="620" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A620" s="8" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B620" s="8" t="s">
         <v>668</v>
@@ -11166,7 +11299,7 @@
     </row>
     <row r="621" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A621" s="8" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B621" s="8" t="s">
         <v>668</v>
@@ -11181,7 +11314,7 @@
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A622" s="8" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B622" s="8" t="s">
         <v>668</v>
@@ -11196,7 +11329,7 @@
     </row>
     <row r="623" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A623" s="19" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B623" s="19" t="s">
         <v>668</v>
@@ -11211,7 +11344,7 @@
     </row>
     <row r="624" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A624" s="19" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B624" s="19" t="s">
         <v>668</v>
@@ -11225,68 +11358,92 @@
       </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A625" s="2"/>
-      <c r="B625" s="2"/>
-      <c r="C625" s="2"/>
-      <c r="D625" s="15">
+      <c r="A625" s="16" t="s">
+        <v>738</v>
+      </c>
+      <c r="B625" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C625" s="16"/>
+      <c r="D625" s="17">
         <v>79</v>
       </c>
-      <c r="E625" s="6" t="s">
+      <c r="E625" s="18" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="626" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A626" s="2"/>
-      <c r="B626" s="2"/>
-      <c r="C626" s="2"/>
-      <c r="D626" s="15">
+      <c r="A626" s="16" t="s">
+        <v>738</v>
+      </c>
+      <c r="B626" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C626" s="16"/>
+      <c r="D626" s="17">
         <v>25</v>
       </c>
-      <c r="E626" s="6" t="s">
+      <c r="E626" s="18" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="627" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A627" s="2"/>
-      <c r="B627" s="2"/>
-      <c r="C627" s="2"/>
-      <c r="D627" s="15">
+      <c r="A627" s="16" t="s">
+        <v>738</v>
+      </c>
+      <c r="B627" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C627" s="16"/>
+      <c r="D627" s="17">
         <v>46</v>
       </c>
-      <c r="E627" s="6" t="s">
+      <c r="E627" s="18" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="628" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A628" s="2"/>
-      <c r="B628" s="2"/>
-      <c r="C628" s="2"/>
-      <c r="D628" s="15">
+      <c r="A628" s="16" t="s">
+        <v>738</v>
+      </c>
+      <c r="B628" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C628" s="16"/>
+      <c r="D628" s="17">
         <v>24</v>
       </c>
-      <c r="E628" s="6" t="s">
+      <c r="E628" s="18" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="629" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A629" s="2"/>
-      <c r="B629" s="2"/>
-      <c r="C629" s="2"/>
-      <c r="D629" s="15">
+      <c r="A629" s="16" t="s">
+        <v>738</v>
+      </c>
+      <c r="B629" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C629" s="16"/>
+      <c r="D629" s="17">
         <v>32</v>
       </c>
-      <c r="E629" s="6" t="s">
+      <c r="E629" s="18" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="630" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A630" s="2"/>
-      <c r="B630" s="2"/>
-      <c r="C630" s="2"/>
-      <c r="D630" s="15">
+      <c r="A630" s="16" t="s">
+        <v>738</v>
+      </c>
+      <c r="B630" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C630" s="16"/>
+      <c r="D630" s="17">
         <v>69</v>
       </c>
-      <c r="E630" s="6" t="s">
+      <c r="E630" s="18" t="s">
         <v>408</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TDrain, TKickout, TLightBargraph, TPopupTarget, TSoloTarget ready.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="744">
   <si>
     <t>Function</t>
   </si>
@@ -2231,6 +2231,21 @@
   </si>
   <si>
     <t>TWall</t>
+  </si>
+  <si>
+    <t>TDrain</t>
+  </si>
+  <si>
+    <t>TKickout</t>
+  </si>
+  <si>
+    <t>TLightBargraph</t>
+  </si>
+  <si>
+    <t>TPopupTarget</t>
+  </si>
+  <si>
+    <t>TSoloTarget</t>
   </si>
 </sst>
 </file>
@@ -2816,7 +2831,7 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:417</v>
+        <v>Done:451</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
@@ -2824,11 +2839,11 @@
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.55391270552053939</v>
+        <v>0.59656296997245639</v>
       </c>
       <c r="E1" s="25" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:53.9999999999999</v>
+        <v>Classes:58.9999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3304,13 +3319,17 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="15">
+      <c r="A35" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20">
         <v>1938</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="21" t="s">
         <v>33</v>
       </c>
     </row>
@@ -7231,13 +7250,17 @@
       </c>
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A324" s="2"/>
-      <c r="B324" s="2"/>
-      <c r="C324" s="2"/>
-      <c r="D324" s="15">
+      <c r="A324" s="8" t="s">
+        <v>700</v>
+      </c>
+      <c r="B324" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C324" s="8"/>
+      <c r="D324" s="13">
         <v>51</v>
       </c>
-      <c r="E324" s="6" t="s">
+      <c r="E324" s="9" t="s">
         <v>144</v>
       </c>
     </row>
@@ -7885,13 +7908,17 @@
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A376" s="2"/>
-      <c r="B376" s="2"/>
-      <c r="C376" s="2"/>
-      <c r="D376" s="15">
+      <c r="A376" s="8" t="s">
+        <v>714</v>
+      </c>
+      <c r="B376" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C376" s="8"/>
+      <c r="D376" s="13">
         <v>93</v>
       </c>
-      <c r="E376" s="6" t="s">
+      <c r="E376" s="9" t="s">
         <v>182</v>
       </c>
     </row>
@@ -8664,46 +8691,62 @@
       </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A435" s="2"/>
-      <c r="B435" s="2"/>
-      <c r="C435" s="2"/>
-      <c r="D435" s="15">
+      <c r="A435" s="19" t="s">
+        <v>739</v>
+      </c>
+      <c r="B435" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C435" s="19"/>
+      <c r="D435" s="20">
         <v>70</v>
       </c>
-      <c r="E435" s="6" t="s">
+      <c r="E435" s="21" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A436" s="2"/>
-      <c r="B436" s="2"/>
-      <c r="C436" s="2"/>
-      <c r="D436" s="15">
+      <c r="A436" s="19" t="s">
+        <v>739</v>
+      </c>
+      <c r="B436" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C436" s="19"/>
+      <c r="D436" s="20">
         <v>48</v>
       </c>
-      <c r="E436" s="6" t="s">
+      <c r="E436" s="21" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A437" s="2"/>
-      <c r="B437" s="2"/>
-      <c r="C437" s="2"/>
-      <c r="D437" s="15">
+      <c r="A437" s="19" t="s">
+        <v>739</v>
+      </c>
+      <c r="B437" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C437" s="19"/>
+      <c r="D437" s="20">
         <v>58</v>
       </c>
-      <c r="E437" s="6" t="s">
+      <c r="E437" s="21" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A438" s="2"/>
-      <c r="B438" s="2"/>
-      <c r="C438" s="2"/>
-      <c r="D438" s="15">
+      <c r="A438" s="19" t="s">
+        <v>739</v>
+      </c>
+      <c r="B438" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C438" s="19"/>
+      <c r="D438" s="20">
         <v>19</v>
       </c>
-      <c r="E438" s="6" t="s">
+      <c r="E438" s="21" t="s">
         <v>227</v>
       </c>
     </row>
@@ -9417,13 +9460,17 @@
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A486" s="2"/>
-      <c r="B486" s="2"/>
-      <c r="C486" s="2"/>
-      <c r="D486" s="15">
+      <c r="A486" s="19" t="s">
+        <v>732</v>
+      </c>
+      <c r="B486" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C486" s="19"/>
+      <c r="D486" s="20">
         <v>111</v>
       </c>
-      <c r="E486" s="6" t="s">
+      <c r="E486" s="21" t="s">
         <v>647</v>
       </c>
     </row>
@@ -9585,90 +9632,122 @@
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A498" s="2"/>
-      <c r="B498" s="2"/>
-      <c r="C498" s="2"/>
-      <c r="D498" s="15">
+      <c r="A498" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="B498" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C498" s="19"/>
+      <c r="D498" s="20">
         <v>116</v>
       </c>
-      <c r="E498" s="6" t="s">
+      <c r="E498" s="21" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="499" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A499" s="2"/>
-      <c r="B499" s="2"/>
-      <c r="C499" s="2"/>
-      <c r="D499" s="15">
+      <c r="A499" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="B499" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C499" s="19"/>
+      <c r="D499" s="20">
         <v>131</v>
       </c>
-      <c r="E499" s="6" t="s">
+      <c r="E499" s="21" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A500" s="2"/>
-      <c r="B500" s="2"/>
-      <c r="C500" s="2"/>
-      <c r="D500" s="15">
+      <c r="A500" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="B500" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C500" s="19"/>
+      <c r="D500" s="20">
         <v>28</v>
       </c>
-      <c r="E500" s="6" t="s">
+      <c r="E500" s="21" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A501" s="2"/>
-      <c r="B501" s="2"/>
-      <c r="C501" s="2"/>
-      <c r="D501" s="15">
+      <c r="A501" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="B501" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C501" s="19"/>
+      <c r="D501" s="20">
         <v>123</v>
       </c>
-      <c r="E501" s="6" t="s">
+      <c r="E501" s="21" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A502" s="2"/>
-      <c r="B502" s="2"/>
-      <c r="C502" s="2"/>
-      <c r="D502" s="15">
+      <c r="A502" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="B502" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C502" s="19"/>
+      <c r="D502" s="20">
         <v>27</v>
       </c>
-      <c r="E502" s="6" t="s">
+      <c r="E502" s="21" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A503" s="2"/>
-      <c r="B503" s="2"/>
-      <c r="C503" s="2"/>
-      <c r="D503" s="15">
+      <c r="A503" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="B503" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C503" s="19"/>
+      <c r="D503" s="20">
         <v>26</v>
       </c>
-      <c r="E503" s="6" t="s">
+      <c r="E503" s="21" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A504" s="2"/>
-      <c r="B504" s="2"/>
-      <c r="C504" s="2"/>
-      <c r="D504" s="15">
+      <c r="A504" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="B504" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C504" s="19"/>
+      <c r="D504" s="20">
         <v>121</v>
       </c>
-      <c r="E504" s="6" t="s">
+      <c r="E504" s="21" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A505" s="2"/>
-      <c r="B505" s="2"/>
-      <c r="C505" s="2"/>
-      <c r="D505" s="15">
+      <c r="A505" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="B505" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C505" s="19"/>
+      <c r="D505" s="20">
         <v>393</v>
       </c>
-      <c r="E505" s="6" t="s">
+      <c r="E505" s="21" t="s">
         <v>283</v>
       </c>
     </row>
@@ -9748,68 +9827,92 @@
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A511" s="2"/>
-      <c r="B511" s="2"/>
-      <c r="C511" s="2"/>
-      <c r="D511" s="15">
+      <c r="A511" s="19" t="s">
+        <v>741</v>
+      </c>
+      <c r="B511" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C511" s="19"/>
+      <c r="D511" s="20">
         <v>33</v>
       </c>
-      <c r="E511" s="6" t="s">
+      <c r="E511" s="21" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A512" s="2"/>
-      <c r="B512" s="2"/>
-      <c r="C512" s="2"/>
-      <c r="D512" s="15">
+      <c r="A512" s="19" t="s">
+        <v>741</v>
+      </c>
+      <c r="B512" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C512" s="19"/>
+      <c r="D512" s="20">
         <v>35</v>
       </c>
-      <c r="E512" s="6" t="s">
+      <c r="E512" s="21" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A513" s="2"/>
-      <c r="B513" s="2"/>
-      <c r="C513" s="2"/>
-      <c r="D513" s="15">
+      <c r="A513" s="19" t="s">
+        <v>741</v>
+      </c>
+      <c r="B513" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C513" s="19"/>
+      <c r="D513" s="20">
         <v>74</v>
       </c>
-      <c r="E513" s="6" t="s">
+      <c r="E513" s="21" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A514" s="2"/>
-      <c r="B514" s="2"/>
-      <c r="C514" s="2"/>
-      <c r="D514" s="15">
+      <c r="A514" s="19" t="s">
+        <v>741</v>
+      </c>
+      <c r="B514" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C514" s="19"/>
+      <c r="D514" s="20">
         <v>454</v>
       </c>
-      <c r="E514" s="6" t="s">
+      <c r="E514" s="21" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A515" s="2"/>
-      <c r="B515" s="2"/>
-      <c r="C515" s="2"/>
-      <c r="D515" s="15">
+      <c r="A515" s="19" t="s">
+        <v>741</v>
+      </c>
+      <c r="B515" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C515" s="19"/>
+      <c r="D515" s="20">
         <v>43</v>
       </c>
-      <c r="E515" s="6" t="s">
+      <c r="E515" s="21" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A516" s="2"/>
-      <c r="B516" s="2"/>
-      <c r="C516" s="2"/>
-      <c r="D516" s="15">
+      <c r="A516" s="19" t="s">
+        <v>741</v>
+      </c>
+      <c r="B516" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C516" s="19"/>
+      <c r="D516" s="20">
         <v>130</v>
       </c>
-      <c r="E516" s="6" t="s">
+      <c r="E516" s="21" t="s">
         <v>295</v>
       </c>
     </row>
@@ -10596,68 +10699,92 @@
       </c>
     </row>
     <row r="569" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A569" s="2"/>
-      <c r="B569" s="2"/>
-      <c r="C569" s="2"/>
-      <c r="D569" s="15">
+      <c r="A569" s="19" t="s">
+        <v>742</v>
+      </c>
+      <c r="B569" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C569" s="19"/>
+      <c r="D569" s="20">
         <v>163</v>
       </c>
-      <c r="E569" s="6" t="s">
+      <c r="E569" s="21" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="570" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A570" s="2"/>
-      <c r="B570" s="2"/>
-      <c r="C570" s="2"/>
-      <c r="D570" s="15">
+      <c r="A570" s="19" t="s">
+        <v>742</v>
+      </c>
+      <c r="B570" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C570" s="19"/>
+      <c r="D570" s="20">
         <v>25</v>
       </c>
-      <c r="E570" s="6" t="s">
+      <c r="E570" s="21" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="571" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A571" s="2"/>
-      <c r="B571" s="2"/>
-      <c r="C571" s="2"/>
-      <c r="D571" s="15">
+      <c r="A571" s="19" t="s">
+        <v>742</v>
+      </c>
+      <c r="B571" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C571" s="19"/>
+      <c r="D571" s="20">
         <v>215</v>
       </c>
-      <c r="E571" s="6" t="s">
+      <c r="E571" s="21" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A572" s="2"/>
-      <c r="B572" s="2"/>
-      <c r="C572" s="2"/>
-      <c r="D572" s="15">
+      <c r="A572" s="19" t="s">
+        <v>742</v>
+      </c>
+      <c r="B572" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C572" s="19"/>
+      <c r="D572" s="20">
         <v>24</v>
       </c>
-      <c r="E572" s="6" t="s">
+      <c r="E572" s="21" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="573" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A573" s="2"/>
-      <c r="B573" s="2"/>
-      <c r="C573" s="2"/>
-      <c r="D573" s="15">
+      <c r="A573" s="19" t="s">
+        <v>742</v>
+      </c>
+      <c r="B573" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C573" s="19"/>
+      <c r="D573" s="20">
         <v>60</v>
       </c>
-      <c r="E573" s="6" t="s">
+      <c r="E573" s="21" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A574" s="2"/>
-      <c r="B574" s="2"/>
-      <c r="C574" s="2"/>
-      <c r="D574" s="15">
+      <c r="A574" s="19" t="s">
+        <v>742</v>
+      </c>
+      <c r="B574" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C574" s="19"/>
+      <c r="D574" s="20">
         <v>58</v>
       </c>
-      <c r="E574" s="6" t="s">
+      <c r="E574" s="21" t="s">
         <v>352</v>
       </c>
     </row>
@@ -10928,68 +11055,92 @@
       </c>
     </row>
     <row r="595" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A595" s="2"/>
-      <c r="B595" s="2"/>
-      <c r="C595" s="2"/>
-      <c r="D595" s="15">
+      <c r="A595" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="B595" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C595" s="19"/>
+      <c r="D595" s="20">
         <v>74</v>
       </c>
-      <c r="E595" s="6" t="s">
+      <c r="E595" s="21" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="596" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A596" s="2"/>
-      <c r="B596" s="2"/>
-      <c r="C596" s="2"/>
-      <c r="D596" s="15">
+      <c r="A596" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="B596" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C596" s="19"/>
+      <c r="D596" s="20">
         <v>25</v>
       </c>
-      <c r="E596" s="6" t="s">
+      <c r="E596" s="21" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="597" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A597" s="2"/>
-      <c r="B597" s="2"/>
-      <c r="C597" s="2"/>
-      <c r="D597" s="15">
+      <c r="A597" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="B597" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C597" s="19"/>
+      <c r="D597" s="20">
         <v>143</v>
       </c>
-      <c r="E597" s="6" t="s">
+      <c r="E597" s="21" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A598" s="2"/>
-      <c r="B598" s="2"/>
-      <c r="C598" s="2"/>
-      <c r="D598" s="15">
+      <c r="A598" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="B598" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C598" s="19"/>
+      <c r="D598" s="20">
         <v>24</v>
       </c>
-      <c r="E598" s="6" t="s">
+      <c r="E598" s="21" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A599" s="2"/>
-      <c r="B599" s="2"/>
-      <c r="C599" s="2"/>
-      <c r="D599" s="15">
+      <c r="A599" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="B599" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C599" s="19"/>
+      <c r="D599" s="20">
         <v>32</v>
       </c>
-      <c r="E599" s="6" t="s">
+      <c r="E599" s="21" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="600" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A600" s="2"/>
-      <c r="B600" s="2"/>
-      <c r="C600" s="2"/>
-      <c r="D600" s="15">
+      <c r="A600" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="B600" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C600" s="19"/>
+      <c r="D600" s="20">
         <v>83</v>
       </c>
-      <c r="E600" s="6" t="s">
+      <c r="E600" s="21" t="s">
         <v>378</v>
       </c>
     </row>

</xml_diff>

<commit_message>
midi ready, TCollision cleanup.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="747">
   <si>
     <t>Function</t>
   </si>
@@ -2252,6 +2252,9 @@
   </si>
   <si>
     <t>TSink</t>
+  </si>
+  <si>
+    <t>midi</t>
   </si>
 </sst>
 </file>
@@ -2837,7 +2840,7 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:574</v>
+        <v>Done:579</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
@@ -2845,11 +2848,11 @@
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.83680021629294177</v>
+        <v>0.83945318440663075</v>
       </c>
       <c r="E1" s="25" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
-        <v>Classes:60.9999999999999</v>
+        <v>Classes:61.9999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -5779,46 +5782,62 @@
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="2"/>
-      <c r="B201" s="2"/>
-      <c r="C201" s="2"/>
-      <c r="D201" s="15">
+      <c r="A201" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C201" s="8"/>
+      <c r="D201" s="13">
         <v>106</v>
       </c>
-      <c r="E201" s="6" t="s">
+      <c r="E201" s="9" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" s="2"/>
-      <c r="B202" s="2"/>
-      <c r="C202" s="2"/>
-      <c r="D202" s="15">
+      <c r="A202" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C202" s="8"/>
+      <c r="D202" s="13">
         <v>38</v>
       </c>
-      <c r="E202" s="6" t="s">
+      <c r="E202" s="9" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" s="2"/>
-      <c r="B203" s="2"/>
-      <c r="C203" s="2"/>
-      <c r="D203" s="15">
+      <c r="A203" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C203" s="8"/>
+      <c r="D203" s="13">
         <v>30</v>
       </c>
-      <c r="E203" s="6" t="s">
+      <c r="E203" s="9" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" s="2"/>
-      <c r="B204" s="2"/>
-      <c r="C204" s="2"/>
-      <c r="D204" s="15">
+      <c r="A204" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C204" s="8"/>
+      <c r="D204" s="13">
         <v>84</v>
       </c>
-      <c r="E204" s="6" t="s">
+      <c r="E204" s="9" t="s">
         <v>530</v>
       </c>
     </row>
@@ -7451,13 +7470,17 @@
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A317" s="2"/>
-      <c r="B317" s="2"/>
-      <c r="C317" s="2"/>
-      <c r="D317" s="15">
+      <c r="A317" s="8" t="s">
+        <v>746</v>
+      </c>
+      <c r="B317" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C317" s="8"/>
+      <c r="D317" s="13">
         <v>56</v>
       </c>
-      <c r="E317" s="6" t="s">
+      <c r="E317" s="9" t="s">
         <v>617</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WaveMix ready. Fixed ball Z reset in TKickout.
</commit_message>
<xml_diff>
--- a/Doc/FuncStats.xlsx
+++ b/Doc/FuncStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="747">
   <si>
     <t>Function</t>
   </si>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="B1" s="3" t="str">
         <f>"Done:"&amp;COUNTIF(B4:B1000,"Done")</f>
-        <v>Done:651</v>
+        <v>Done:656</v>
       </c>
       <c r="C1" s="3" t="str">
         <f>"Inp:"&amp;COUNTIF(B4:B1000,"Inp")</f>
@@ -2848,7 +2848,7 @@
       </c>
       <c r="D1" s="12">
         <f>SUMIF(B4:B1000,{"Done","Inp"},D4:D1000) / SUM(D4:D1000)</f>
-        <v>0.97205934537589345</v>
+        <v>0.98376958042548879</v>
       </c>
       <c r="E1" s="25" t="str">
         <f t="array" ref="E1">"Classes:"&amp;SUM(IF(A4:A1000&lt;&gt;"",1/COUNTIF(A4:A1000, A4:A1000), 0))</f>
@@ -4144,7 +4144,9 @@
       <c r="A86" s="16" t="s">
         <v>746</v>
       </c>
-      <c r="B86" s="16"/>
+      <c r="B86" s="16" t="s">
+        <v>668</v>
+      </c>
       <c r="C86" s="16"/>
       <c r="D86" s="17">
         <v>204</v>
@@ -4813,28 +4815,32 @@
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="16" t="s">
+      <c r="A130" s="19" t="s">
         <v>679</v>
       </c>
-      <c r="B130" s="16" t="s">
-        <v>668</v>
-      </c>
-      <c r="C130" s="16"/>
-      <c r="D130" s="17">
+      <c r="B130" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="C130" s="19"/>
+      <c r="D130" s="20">
         <v>63</v>
       </c>
-      <c r="E130" s="18" t="s">
+      <c r="E130" s="21" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="15">
+      <c r="A131" s="16" t="s">
+        <v>746</v>
+      </c>
+      <c r="B131" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C131" s="16"/>
+      <c r="D131" s="17">
         <v>22</v>
       </c>
-      <c r="E131" s="6" t="s">
+      <c r="E131" s="18" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4914,13 +4920,17 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="15">
+      <c r="A137" s="16" t="s">
+        <v>746</v>
+      </c>
+      <c r="B137" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C137" s="16"/>
+      <c r="D137" s="17">
         <v>38</v>
       </c>
-      <c r="E137" s="6" t="s">
+      <c r="E137" s="18" t="s">
         <v>82</v>
       </c>
     </row>
@@ -7601,13 +7611,17 @@
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A316" s="2"/>
-      <c r="B316" s="2"/>
-      <c r="C316" s="2"/>
-      <c r="D316" s="15">
+      <c r="A316" s="16" t="s">
+        <v>746</v>
+      </c>
+      <c r="B316" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C316" s="16"/>
+      <c r="D316" s="17">
         <v>49</v>
       </c>
-      <c r="E316" s="6" t="s">
+      <c r="E316" s="18" t="s">
         <v>137</v>
       </c>
     </row>
@@ -12624,7 +12638,9 @@
       <c r="A652" s="16" t="s">
         <v>746</v>
       </c>
-      <c r="B652" s="16"/>
+      <c r="B652" s="16" t="s">
+        <v>668</v>
+      </c>
       <c r="C652" s="16"/>
       <c r="D652" s="17">
         <v>1073</v>

</xml_diff>